<commit_message>
2021 Q1 update, fixed some issues in data_prep.py where quarters and months beyond the scope of the current update were being included in the results.
</commit_message>
<xml_diff>
--- a/web_files/US State Power Sector CO2 Emissions.xlsx
+++ b/web_files/US State Power Sector CO2 Emissions.xlsx
@@ -853,7 +853,7 @@
         <v>122569670</v>
       </c>
       <c r="E16" t="n">
-        <v>971.2554529537363</v>
+        <v>971.2554529537364</v>
       </c>
       <c r="F16" t="n">
         <v>2141.229771581807</v>
@@ -1733,7 +1733,7 @@
         <v>203352778</v>
       </c>
       <c r="E60" t="n">
-        <v>607.0440914077899</v>
+        <v>607.0440914077898</v>
       </c>
       <c r="F60" t="n">
         <v>1338.289403917614</v>
@@ -2173,10 +2173,10 @@
         <v>61569386</v>
       </c>
       <c r="E82" t="n">
-        <v>334.0726153689432</v>
+        <v>334.0726153689433</v>
       </c>
       <c r="F82" t="n">
-        <v>736.4964878423723</v>
+        <v>736.4964878423724</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -5887,13 +5887,13 @@
         <v>22</v>
       </c>
       <c r="C268" t="n">
-        <v>94149286621.13</v>
+        <v>94149286621.12999</v>
       </c>
       <c r="D268" t="n">
         <v>98792014.20000002</v>
       </c>
       <c r="E268" t="n">
-        <v>953.0050316671243</v>
+        <v>953.0050316671241</v>
       </c>
       <c r="F268" t="n">
         <v>2100.994892813342</v>
@@ -6053,7 +6053,7 @@
         <v>46228847.42</v>
       </c>
       <c r="E276" t="n">
-        <v>554.9665658524307</v>
+        <v>554.9665658524308</v>
       </c>
       <c r="F276" t="n">
         <v>1223.479291078269</v>
@@ -6987,13 +6987,13 @@
         <v>27</v>
       </c>
       <c r="C323" t="n">
-        <v>76430491605.26999</v>
+        <v>76430491605.27</v>
       </c>
       <c r="D323" t="n">
         <v>119309936.25</v>
       </c>
       <c r="E323" t="n">
-        <v>640.6045800336263</v>
+        <v>640.6045800336266</v>
       </c>
       <c r="F323" t="n">
         <v>1412.276857142133</v>
@@ -7047,13 +7047,13 @@
         <v>30</v>
       </c>
       <c r="C326" t="n">
-        <v>27568366764.73001</v>
+        <v>27568366764.73</v>
       </c>
       <c r="D326" t="n">
         <v>50043685.98</v>
       </c>
       <c r="E326" t="n">
-        <v>550.8860153855919</v>
+        <v>550.8860153855918</v>
       </c>
       <c r="F326" t="n">
         <v>1214.483309519076</v>
@@ -7853,10 +7853,10 @@
         <v>129510294.01</v>
       </c>
       <c r="E366" t="n">
-        <v>968.0084813712562</v>
+        <v>968.0084813712563</v>
       </c>
       <c r="F366" t="n">
-        <v>2134.071498031071</v>
+        <v>2134.071498031072</v>
       </c>
     </row>
     <row r="367" spans="1:6">
@@ -9987,13 +9987,13 @@
         <v>27</v>
       </c>
       <c r="C473" t="n">
-        <v>71811440416.83998</v>
+        <v>71811440416.84</v>
       </c>
       <c r="D473" t="n">
         <v>111551371.35</v>
       </c>
       <c r="E473" t="n">
-        <v>643.7521972860981</v>
+        <v>643.7521972860982</v>
       </c>
       <c r="F473" t="n">
         <v>1419.216094136932</v>
@@ -10013,7 +10013,7 @@
         <v>53670227.02999999</v>
       </c>
       <c r="E474" t="n">
-        <v>585.0274667584168</v>
+        <v>585.0274667584169</v>
       </c>
       <c r="F474" t="n">
         <v>1289.751553215606</v>
@@ -11113,7 +11113,7 @@
         <v>35079900.14000001</v>
       </c>
       <c r="E529" t="n">
-        <v>841.6477784246621</v>
+        <v>841.6477784246622</v>
       </c>
       <c r="F529" t="n">
         <v>1855.49669231501</v>
@@ -16907,16 +16907,16 @@
         <v>23</v>
       </c>
       <c r="C819" t="n">
-        <v>40160780663.57802</v>
+        <v>40160796865.89676</v>
       </c>
       <c r="D819" t="n">
         <v>97916675.57999998</v>
       </c>
       <c r="E819" t="n">
-        <v>410.1526162493723</v>
+        <v>410.1527817198465</v>
       </c>
       <c r="F819" t="n">
-        <v>904.2224577833663</v>
+        <v>904.2228225795737</v>
       </c>
     </row>
     <row r="820" spans="1:6">
@@ -17787,13 +17787,13 @@
         <v>17</v>
       </c>
       <c r="C863" t="n">
-        <v>30700167574.87014</v>
+        <v>30700167574.87012</v>
       </c>
       <c r="D863" t="n">
         <v>63506748.48999999</v>
       </c>
       <c r="E863" t="n">
-        <v>483.4158306767083</v>
+        <v>483.4158306767081</v>
       </c>
       <c r="F863" t="n">
         <v>1065.738540309871</v>
@@ -17907,16 +17907,16 @@
         <v>23</v>
       </c>
       <c r="C869" t="n">
-        <v>40594233400.4137</v>
+        <v>40594479546.83835</v>
       </c>
       <c r="D869" t="n">
         <v>102357107.35</v>
       </c>
       <c r="E869" t="n">
-        <v>396.5941833585208</v>
+        <v>396.5965881394982</v>
       </c>
       <c r="F869" t="n">
-        <v>874.331536632195</v>
+        <v>874.3368382123377</v>
       </c>
     </row>
     <row r="870" spans="1:6">
@@ -17947,16 +17947,16 @@
         <v>25</v>
       </c>
       <c r="C871" t="n">
-        <v>16747461766.57892</v>
+        <v>16743252678.73892</v>
       </c>
       <c r="D871" t="n">
         <v>44658475.45</v>
       </c>
       <c r="E871" t="n">
-        <v>375.0119456121945</v>
+        <v>374.9176950181564</v>
       </c>
       <c r="F871" t="n">
-        <v>826.751335296644</v>
+        <v>826.5435504370276</v>
       </c>
     </row>
     <row r="872" spans="1:6">

</xml_diff>

<commit_message>
2021 Q3 update. No changes to the code.
</commit_message>
<xml_diff>
--- a/web_files/US State Power Sector CO2 Emissions.xlsx
+++ b/web_files/US State Power Sector CO2 Emissions.xlsx
@@ -853,7 +853,7 @@
         <v>122569670</v>
       </c>
       <c r="E16" t="n">
-        <v>971.2554529537363</v>
+        <v>971.2554529537364</v>
       </c>
       <c r="F16" t="n">
         <v>2141.229771581807</v>
@@ -953,7 +953,7 @@
         <v>49062342</v>
       </c>
       <c r="E21" t="n">
-        <v>654.920077338644</v>
+        <v>654.9200773386441</v>
       </c>
       <c r="F21" t="n">
         <v>1443.836802500775</v>
@@ -2173,10 +2173,10 @@
         <v>61569386</v>
       </c>
       <c r="E82" t="n">
-        <v>334.0726153689433</v>
+        <v>334.0726153689432</v>
       </c>
       <c r="F82" t="n">
-        <v>736.4964878423724</v>
+        <v>736.4964878423723</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3907,13 +3907,13 @@
         <v>23</v>
       </c>
       <c r="C169" t="n">
-        <v>50732697297.7825</v>
+        <v>50732697297.78251</v>
       </c>
       <c r="D169" t="n">
         <v>98172308.65000001</v>
       </c>
       <c r="E169" t="n">
-        <v>516.7719695647852</v>
+        <v>516.7719695647853</v>
       </c>
       <c r="F169" t="n">
         <v>1139.275484102526</v>
@@ -6027,13 +6027,13 @@
         <v>29</v>
       </c>
       <c r="C275" t="n">
-        <v>79695807549.96605</v>
+        <v>79695807549.96606</v>
       </c>
       <c r="D275" t="n">
         <v>91686342.91</v>
       </c>
       <c r="E275" t="n">
-        <v>869.2222311472937</v>
+        <v>869.2222311472939</v>
       </c>
       <c r="F275" t="n">
         <v>1916.287330787324</v>
@@ -8667,16 +8667,16 @@
         <v>11</v>
       </c>
       <c r="C407" t="n">
-        <v>38405119201.1</v>
+        <v>38405119201.09999</v>
       </c>
       <c r="D407" t="n">
         <v>50565951.61000001</v>
       </c>
       <c r="E407" t="n">
-        <v>759.5055166232634</v>
+        <v>759.5055166232632</v>
       </c>
       <c r="F407" t="n">
-        <v>1674.405861947647</v>
+        <v>1674.405861947646</v>
       </c>
     </row>
     <row r="408" spans="1:6">
@@ -8687,16 +8687,16 @@
         <v>12</v>
       </c>
       <c r="C408" t="n">
-        <v>7514791746.705</v>
+        <v>7514791746.705002</v>
       </c>
       <c r="D408" t="n">
         <v>31206222.07</v>
       </c>
       <c r="E408" t="n">
-        <v>240.8106860820336</v>
+        <v>240.8106860820337</v>
       </c>
       <c r="F408" t="n">
-        <v>530.8912385364513</v>
+        <v>530.8912385364515</v>
       </c>
     </row>
     <row r="409" spans="1:6">
@@ -8887,16 +8887,16 @@
         <v>22</v>
       </c>
       <c r="C418" t="n">
-        <v>86092205729.145</v>
+        <v>86092205729.14499</v>
       </c>
       <c r="D418" t="n">
         <v>90630426.69000001</v>
       </c>
       <c r="E418" t="n">
-        <v>949.9260775150279</v>
+        <v>949.9260775150277</v>
       </c>
       <c r="F418" t="n">
-        <v>2094.207030489631</v>
+        <v>2094.20703048963</v>
       </c>
     </row>
     <row r="419" spans="1:6">
@@ -10013,7 +10013,7 @@
         <v>53670227.02999999</v>
       </c>
       <c r="E474" t="n">
-        <v>585.0274667584168</v>
+        <v>585.0274667584169</v>
       </c>
       <c r="F474" t="n">
         <v>1289.751553215606</v>
@@ -10733,10 +10733,10 @@
         <v>221923641.13</v>
       </c>
       <c r="E510" t="n">
-        <v>504.7993257629822</v>
+        <v>504.7993257629821</v>
       </c>
       <c r="F510" t="n">
-        <v>1112.880593577071</v>
+        <v>1112.88059357707</v>
       </c>
     </row>
     <row r="511" spans="1:6">
@@ -14230,13 +14230,13 @@
         <v>33340263073.56986</v>
       </c>
       <c r="D685" t="n">
-        <v>137472361.41</v>
+        <v>137427471.44</v>
       </c>
       <c r="E685" t="n">
-        <v>242.5233896589241</v>
+        <v>242.6026086649351</v>
       </c>
       <c r="F685" t="n">
-        <v>534.6670648420641</v>
+        <v>534.8417110627161</v>
       </c>
     </row>
     <row r="686" spans="1:6">
@@ -14310,13 +14310,13 @@
         <v>99519921237.6973</v>
       </c>
       <c r="D689" t="n">
-        <v>221310099.17</v>
+        <v>221286968.17</v>
       </c>
       <c r="E689" t="n">
-        <v>449.6854034720339</v>
+        <v>449.7324088296187</v>
       </c>
       <c r="F689" t="n">
-        <v>991.376440494446</v>
+        <v>991.4800685057776</v>
       </c>
     </row>
     <row r="690" spans="1:6">
@@ -15230,13 +15230,13 @@
         <v>32304043655.07257</v>
       </c>
       <c r="D735" t="n">
-        <v>139216237.11</v>
+        <v>139170202.12</v>
       </c>
       <c r="E735" t="n">
-        <v>232.0422123573699</v>
+        <v>232.1189677314566</v>
       </c>
       <c r="F735" t="n">
-        <v>511.5602613630576</v>
+        <v>511.7294762607692</v>
       </c>
     </row>
     <row r="736" spans="1:6">
@@ -15310,13 +15310,13 @@
         <v>89658007195.42918</v>
       </c>
       <c r="D739" t="n">
-        <v>214833642.73</v>
+        <v>214806618.75</v>
       </c>
       <c r="E739" t="n">
-        <v>417.3369033643867</v>
+        <v>417.3894068868358</v>
       </c>
       <c r="F739" t="n">
-        <v>920.0609371571269</v>
+        <v>920.1766864227184</v>
       </c>
     </row>
     <row r="740" spans="1:6">
@@ -16156,7 +16156,7 @@
         <v>125.6231856594525</v>
       </c>
       <c r="F781" t="n">
-        <v>276.9488751048291</v>
+        <v>276.948875104829</v>
       </c>
     </row>
     <row r="782" spans="1:6">
@@ -16230,13 +16230,13 @@
         <v>29887152843.38305</v>
       </c>
       <c r="D785" t="n">
-        <v>135290536.33</v>
+        <v>135250144.35</v>
       </c>
       <c r="E785" t="n">
-        <v>220.9108904002159</v>
+        <v>220.9768646607958</v>
       </c>
       <c r="F785" t="n">
-        <v>487.0201489763159</v>
+        <v>487.1655958311905</v>
       </c>
     </row>
     <row r="786" spans="1:6">
@@ -16310,13 +16310,13 @@
         <v>83808466141.26736</v>
       </c>
       <c r="D789" t="n">
-        <v>215353023.99</v>
+        <v>215328245.01</v>
       </c>
       <c r="E789" t="n">
-        <v>389.1678165854733</v>
+        <v>389.2126002205388</v>
       </c>
       <c r="F789" t="n">
-        <v>857.9593684443345</v>
+        <v>858.0580984461998</v>
       </c>
     </row>
     <row r="790" spans="1:6">
@@ -16487,16 +16487,16 @@
         <v>52</v>
       </c>
       <c r="C798" t="n">
-        <v>9562590002.616528</v>
+        <v>9580492180.462585</v>
       </c>
       <c r="D798" t="n">
         <v>114175913.16</v>
       </c>
       <c r="E798" t="n">
-        <v>83.75312916670985</v>
+        <v>83.90992386491359</v>
       </c>
       <c r="F798" t="n">
-        <v>184.6421485609285</v>
+        <v>184.9878181525885</v>
       </c>
     </row>
     <row r="799" spans="1:6">
@@ -17007,16 +17007,16 @@
         <v>28</v>
       </c>
       <c r="C824" t="n">
-        <v>26779115853.183</v>
+        <v>26779197207.103</v>
       </c>
       <c r="D824" t="n">
         <v>58807433.09</v>
       </c>
       <c r="E824" t="n">
-        <v>455.3695756827158</v>
+        <v>455.3709590779045</v>
       </c>
       <c r="F824" t="n">
-        <v>1003.907766550115</v>
+        <v>1003.910816383148</v>
       </c>
     </row>
     <row r="825" spans="1:6">
@@ -17230,13 +17230,13 @@
         <v>24191103650.96247</v>
       </c>
       <c r="D835" t="n">
-        <v>129246657.48</v>
+        <v>129206961.49</v>
       </c>
       <c r="E835" t="n">
-        <v>187.1700523837985</v>
+        <v>187.2275562554325</v>
       </c>
       <c r="F835" t="n">
-        <v>412.6350974853223</v>
+        <v>412.7618705207264</v>
       </c>
     </row>
     <row r="836" spans="1:6">
@@ -17310,13 +17310,13 @@
         <v>79073163869.04344</v>
       </c>
       <c r="D839" t="n">
-        <v>213996704.1</v>
+        <v>213948699.11</v>
       </c>
       <c r="E839" t="n">
-        <v>369.5064566606259</v>
+        <v>369.5893651047097</v>
       </c>
       <c r="F839" t="n">
-        <v>814.613934354016</v>
+        <v>814.796714309843</v>
       </c>
     </row>
     <row r="840" spans="1:6">
@@ -17407,16 +17407,16 @@
         <v>48</v>
       </c>
       <c r="C844" t="n">
-        <v>220418542510.8158</v>
+        <v>220413738134.1266</v>
       </c>
       <c r="D844" t="n">
         <v>453270703.1300001</v>
       </c>
       <c r="E844" t="n">
-        <v>486.2845557604874</v>
+        <v>486.2739564063793</v>
       </c>
       <c r="F844" t="n">
-        <v>1072.062931629571</v>
+        <v>1072.039564293504</v>
       </c>
     </row>
     <row r="845" spans="1:6">
@@ -17487,16 +17487,16 @@
         <v>52</v>
       </c>
       <c r="C848" t="n">
-        <v>10420289431.51407</v>
+        <v>10425338770.75192</v>
       </c>
       <c r="D848" t="n">
         <v>116027998.89</v>
       </c>
       <c r="E848" t="n">
-        <v>89.80840427484223</v>
+        <v>89.85192255737887</v>
       </c>
       <c r="F848" t="n">
-        <v>197.9916080643172</v>
+        <v>198.0875484699975</v>
       </c>
     </row>
     <row r="849" spans="1:6">
@@ -17787,7 +17787,7 @@
         <v>17</v>
       </c>
       <c r="C863" t="n">
-        <v>30700167574.87013</v>
+        <v>30700167574.87012</v>
       </c>
       <c r="D863" t="n">
         <v>63506748.48999999</v>
@@ -18007,16 +18007,16 @@
         <v>28</v>
       </c>
       <c r="C874" t="n">
-        <v>27964625062.01057</v>
+        <v>27964738094.21056</v>
       </c>
       <c r="D874" t="n">
         <v>61598169.68000001</v>
       </c>
       <c r="E874" t="n">
-        <v>453.9846753123617</v>
+        <v>453.9865103051965</v>
       </c>
       <c r="F874" t="n">
-        <v>1000.854615193633</v>
+        <v>1000.858660618836</v>
       </c>
     </row>
     <row r="875" spans="1:6">
@@ -18407,16 +18407,16 @@
         <v>48</v>
       </c>
       <c r="C894" t="n">
-        <v>211867781160.6168</v>
+        <v>211857038907.1713</v>
       </c>
       <c r="D894" t="n">
         <v>478068089.03</v>
       </c>
       <c r="E894" t="n">
-        <v>443.1749075544793</v>
+        <v>443.1524374216842</v>
       </c>
       <c r="F894" t="n">
-        <v>977.0234011946051</v>
+        <v>976.9738635398451</v>
       </c>
     </row>
     <row r="895" spans="1:6">
@@ -18487,16 +18487,16 @@
         <v>52</v>
       </c>
       <c r="C898" t="n">
-        <v>10351478611.95705</v>
+        <v>10368479928.18046</v>
       </c>
       <c r="D898" t="n">
         <v>116906292.69</v>
       </c>
       <c r="E898" t="n">
-        <v>88.54509345708215</v>
+        <v>88.69052032703257</v>
       </c>
       <c r="F898" t="n">
-        <v>195.2065130354833</v>
+        <v>195.527121112976</v>
       </c>
     </row>
     <row r="899" spans="1:6">
@@ -19007,16 +19007,16 @@
         <v>28</v>
       </c>
       <c r="C924" t="n">
-        <v>23939993325.19771</v>
+        <v>23940638084.27771</v>
       </c>
       <c r="D924" t="n">
         <v>59483688.84</v>
       </c>
       <c r="E924" t="n">
-        <v>402.4631590954591</v>
+        <v>402.4739983539613</v>
       </c>
       <c r="F924" t="n">
-        <v>887.2702805418492</v>
+        <v>887.2941767711432</v>
       </c>
     </row>
     <row r="925" spans="1:6">
@@ -19407,16 +19407,16 @@
         <v>48</v>
       </c>
       <c r="C944" t="n">
-        <v>198980412292.8443</v>
+        <v>198985482066.4175</v>
       </c>
       <c r="D944" t="n">
         <v>484201997.66</v>
       </c>
       <c r="E944" t="n">
-        <v>410.9450461882761</v>
+        <v>410.9555165572497</v>
       </c>
       <c r="F944" t="n">
-        <v>905.9694488266734</v>
+        <v>905.9925318021127</v>
       </c>
     </row>
     <row r="945" spans="1:6">
@@ -19487,16 +19487,16 @@
         <v>52</v>
       </c>
       <c r="C948" t="n">
-        <v>14275790278.54039</v>
+        <v>14309587138.81765</v>
       </c>
       <c r="D948" t="n">
         <v>106668341.34</v>
       </c>
       <c r="E948" t="n">
-        <v>133.8334326680587</v>
+        <v>134.1502732587409</v>
       </c>
       <c r="F948" t="n">
-        <v>295.0491856600023</v>
+        <v>295.7476924262202</v>
       </c>
     </row>
     <row r="949" spans="1:6">
@@ -19567,16 +19567,16 @@
         <v>6</v>
       </c>
       <c r="C952" t="n">
-        <v>2584550899.445</v>
+        <v>2808334799.155</v>
       </c>
       <c r="D952" t="n">
-        <v>5898991.86</v>
+        <v>6283164.9</v>
       </c>
       <c r="E952" t="n">
-        <v>438.1343390165316</v>
+        <v>446.9618168313551</v>
       </c>
       <c r="F952" t="n">
-        <v>965.9109637958455</v>
+        <v>985.3720213864055</v>
       </c>
     </row>
     <row r="953" spans="1:6">
@@ -19587,16 +19587,16 @@
         <v>7</v>
       </c>
       <c r="C953" t="n">
-        <v>44472448824.8619</v>
+        <v>42560364927.26501</v>
       </c>
       <c r="D953" t="n">
-        <v>135865961.55</v>
+        <v>137542701.67</v>
       </c>
       <c r="E953" t="n">
-        <v>327.3259050133436</v>
+        <v>309.43382971623</v>
       </c>
       <c r="F953" t="n">
-        <v>721.6226901924174</v>
+        <v>682.1778209924008</v>
       </c>
     </row>
     <row r="954" spans="1:6">
@@ -19607,16 +19607,16 @@
         <v>8</v>
       </c>
       <c r="C954" t="n">
-        <v>23299832052.79658</v>
+        <v>22605591632.085</v>
       </c>
       <c r="D954" t="n">
-        <v>53026769.22</v>
+        <v>54727500.27999999</v>
       </c>
       <c r="E954" t="n">
-        <v>439.3975419495976</v>
+        <v>413.0572658431131</v>
       </c>
       <c r="F954" t="n">
-        <v>968.695820982083</v>
+        <v>910.6260482777271</v>
       </c>
     </row>
     <row r="955" spans="1:6">
@@ -19627,16 +19627,16 @@
         <v>9</v>
       </c>
       <c r="C955" t="n">
-        <v>40132962486.93383</v>
+        <v>35708721850.66</v>
       </c>
       <c r="D955" t="n">
-        <v>113262931.66</v>
+        <v>112992809.25</v>
       </c>
       <c r="E955" t="n">
-        <v>354.3344843607576</v>
+        <v>316.0264983911798</v>
       </c>
       <c r="F955" t="n">
-        <v>781.1658042217263</v>
+        <v>696.7120183531949</v>
       </c>
     </row>
     <row r="956" spans="1:6">
@@ -19647,16 +19647,16 @@
         <v>10</v>
       </c>
       <c r="C956" t="n">
-        <v>38579055002.29417</v>
+        <v>37774782667.21999</v>
       </c>
       <c r="D956" t="n">
-        <v>213828187.49</v>
+        <v>212702187.88</v>
       </c>
       <c r="E956" t="n">
-        <v>180.420811003219</v>
+        <v>177.5947066822433</v>
       </c>
       <c r="F956" t="n">
-        <v>397.7557199376967</v>
+        <v>391.5252903516736</v>
       </c>
     </row>
     <row r="957" spans="1:6">
@@ -19667,16 +19667,16 @@
         <v>11</v>
       </c>
       <c r="C957" t="n">
-        <v>29668002872.75095</v>
+        <v>28892082200.82</v>
       </c>
       <c r="D957" t="n">
-        <v>54899372.40000001</v>
+        <v>54815696.35</v>
       </c>
       <c r="E957" t="n">
-        <v>540.4069586914067</v>
+        <v>527.0768069120771</v>
       </c>
       <c r="F957" t="n">
-        <v>1191.381181131075</v>
+        <v>1161.993528518365</v>
       </c>
     </row>
     <row r="958" spans="1:6">
@@ -19687,16 +19687,16 @@
         <v>12</v>
       </c>
       <c r="C958" t="n">
-        <v>9862371713.702158</v>
+        <v>9972877697.759998</v>
       </c>
       <c r="D958" t="n">
-        <v>41761807.04</v>
+        <v>41925724.74</v>
       </c>
       <c r="E958" t="n">
-        <v>236.1576859989763</v>
+        <v>237.8701324689372</v>
       </c>
       <c r="F958" t="n">
-        <v>520.6332345533432</v>
+        <v>524.408494041019</v>
       </c>
     </row>
     <row r="959" spans="1:6">
@@ -19707,16 +19707,16 @@
         <v>13</v>
       </c>
       <c r="C959" t="n">
-        <v>1692476585.791443</v>
+        <v>2079263866.375</v>
       </c>
       <c r="D959" t="n">
-        <v>5139553.060000001</v>
+        <v>5333805.300000001</v>
       </c>
       <c r="E959" t="n">
-        <v>329.3042344408528</v>
+        <v>389.8274776499621</v>
       </c>
       <c r="F959" t="n">
-        <v>725.9841152483042</v>
+        <v>859.4136572271066</v>
       </c>
     </row>
     <row r="960" spans="1:6">
@@ -19727,16 +19727,16 @@
         <v>14</v>
       </c>
       <c r="C960" t="n">
-        <v>95205331494.32219</v>
+        <v>95440192441.855</v>
       </c>
       <c r="D960" t="n">
-        <v>250710680.8500001</v>
+        <v>251974893.25</v>
       </c>
       <c r="E960" t="n">
-        <v>379.7418250053872</v>
+        <v>378.7686590947885</v>
       </c>
       <c r="F960" t="n">
-        <v>837.1788274068766</v>
+        <v>835.0333858403708</v>
       </c>
     </row>
     <row r="961" spans="1:6">
@@ -19747,16 +19747,16 @@
         <v>15</v>
       </c>
       <c r="C961" t="n">
-        <v>38841786515.80583</v>
+        <v>37730463955.495</v>
       </c>
       <c r="D961" t="n">
-        <v>119360107.44</v>
+        <v>120326774.35</v>
       </c>
       <c r="E961" t="n">
-        <v>325.4168193115178</v>
+        <v>313.5666534677201</v>
       </c>
       <c r="F961" t="n">
-        <v>717.4139198541723</v>
+        <v>691.2890442349359</v>
       </c>
     </row>
     <row r="962" spans="1:6">
@@ -19767,16 +19767,16 @@
         <v>16</v>
       </c>
       <c r="C962" t="n">
-        <v>6527311567.155001</v>
+        <v>6535712231.1</v>
       </c>
       <c r="D962" t="n">
-        <v>10258431.12</v>
+        <v>10289725.16</v>
       </c>
       <c r="E962" t="n">
-        <v>636.2875073976226</v>
+        <v>635.1687853147674</v>
       </c>
       <c r="F962" t="n">
-        <v>1402.759438808799</v>
+        <v>1400.293104104936</v>
       </c>
     </row>
     <row r="963" spans="1:6">
@@ -19787,16 +19787,16 @@
         <v>17</v>
       </c>
       <c r="C963" t="n">
-        <v>16725866015.13769</v>
+        <v>16296664463.41</v>
       </c>
       <c r="D963" t="n">
-        <v>59497482.68</v>
+        <v>59846494.78</v>
       </c>
       <c r="E963" t="n">
-        <v>281.118885400509</v>
+        <v>272.3077520800125</v>
       </c>
       <c r="F963" t="n">
-        <v>619.7546947539621</v>
+        <v>600.3296702355956</v>
       </c>
     </row>
     <row r="964" spans="1:6">
@@ -19807,16 +19807,16 @@
         <v>18</v>
       </c>
       <c r="C964" t="n">
-        <v>1601968448.482061</v>
+        <v>1708644232.975</v>
       </c>
       <c r="D964" t="n">
-        <v>19388128.55</v>
+        <v>17773269.45</v>
       </c>
       <c r="E964" t="n">
-        <v>82.62625473885981</v>
+        <v>96.13561746654327</v>
       </c>
       <c r="F964" t="n">
-        <v>182.1578411972904</v>
+        <v>211.9405822667413</v>
       </c>
     </row>
     <row r="965" spans="1:6">
@@ -19827,16 +19827,16 @@
         <v>19</v>
       </c>
       <c r="C965" t="n">
-        <v>43209972681.16507</v>
+        <v>43331370870.71499</v>
       </c>
       <c r="D965" t="n">
-        <v>173943358.18</v>
+        <v>173821585.18</v>
       </c>
       <c r="E965" t="n">
-        <v>248.4140419805541</v>
+        <v>249.2864785799958</v>
       </c>
       <c r="F965" t="n">
-        <v>547.6535969503295</v>
+        <v>549.5769706774588</v>
       </c>
     </row>
     <row r="966" spans="1:6">
@@ -19847,16 +19847,16 @@
         <v>20</v>
       </c>
       <c r="C966" t="n">
-        <v>62955464856.34379</v>
+        <v>63967371194.355</v>
       </c>
       <c r="D966" t="n">
-        <v>89906922.03</v>
+        <v>90240205.28999998</v>
       </c>
       <c r="E966" t="n">
-        <v>700.2293420225965</v>
+        <v>708.8566674775016</v>
       </c>
       <c r="F966" t="n">
-        <v>1543.725607423016</v>
+        <v>1562.7454091209</v>
       </c>
     </row>
     <row r="967" spans="1:6">
@@ -19867,16 +19867,16 @@
         <v>21</v>
       </c>
       <c r="C967" t="n">
-        <v>19858526191.73903</v>
+        <v>20157001750.585</v>
       </c>
       <c r="D967" t="n">
-        <v>54387390.53</v>
+        <v>54589706.59999999</v>
       </c>
       <c r="E967" t="n">
-        <v>365.1310717101807</v>
+        <v>369.2454678000596</v>
       </c>
       <c r="F967" t="n">
-        <v>804.9679606922645</v>
+        <v>814.0385583120114</v>
       </c>
     </row>
     <row r="968" spans="1:6">
@@ -19887,16 +19887,16 @@
         <v>22</v>
       </c>
       <c r="C968" t="n">
-        <v>48559338876.30147</v>
+        <v>49247599870.59</v>
       </c>
       <c r="D968" t="n">
-        <v>63475218.50000001</v>
+        <v>63590731.15000001</v>
       </c>
       <c r="E968" t="n">
-        <v>765.0125517299552</v>
+        <v>774.446196481419</v>
       </c>
       <c r="F968" t="n">
-        <v>1686.546671543859</v>
+        <v>1707.344084762936</v>
       </c>
     </row>
     <row r="969" spans="1:6">
@@ -19907,16 +19907,16 @@
         <v>23</v>
       </c>
       <c r="C969" t="n">
-        <v>35198014991.9602</v>
+        <v>36052740045.305</v>
       </c>
       <c r="D969" t="n">
-        <v>102245364.44</v>
+        <v>101030769.69</v>
       </c>
       <c r="E969" t="n">
-        <v>344.2504722315819</v>
+        <v>356.8491080086613</v>
       </c>
       <c r="F969" t="n">
-        <v>758.9345910817453</v>
+        <v>786.7095435158949</v>
       </c>
     </row>
     <row r="970" spans="1:6">
@@ -19927,16 +19927,16 @@
         <v>24</v>
       </c>
       <c r="C970" t="n">
-        <v>6991457674.526141</v>
+        <v>7183269475.57</v>
       </c>
       <c r="D970" t="n">
-        <v>20619433.35</v>
+        <v>20535999.84</v>
       </c>
       <c r="E970" t="n">
-        <v>339.071280759815</v>
+        <v>349.7891279478116</v>
       </c>
       <c r="F970" t="n">
-        <v>747.5165455630881</v>
+        <v>771.1451114737455</v>
       </c>
     </row>
     <row r="971" spans="1:6">
@@ -19947,16 +19947,16 @@
         <v>25</v>
       </c>
       <c r="C971" t="n">
-        <v>10536438538.04916</v>
+        <v>9777720690.965</v>
       </c>
       <c r="D971" t="n">
-        <v>37072371.36000001</v>
+        <v>37023543.94</v>
       </c>
       <c r="E971" t="n">
-        <v>284.212694023066</v>
+        <v>264.094671942013</v>
       </c>
       <c r="F971" t="n">
-        <v>626.5753052432514</v>
+        <v>582.2231137633618</v>
       </c>
     </row>
     <row r="972" spans="1:6">
@@ -19967,16 +19967,16 @@
         <v>26</v>
       </c>
       <c r="C972" t="n">
-        <v>981543254.49993</v>
+        <v>989074059.7849998</v>
       </c>
       <c r="D972" t="n">
-        <v>10490609.68</v>
+        <v>10090930.08</v>
       </c>
       <c r="E972" t="n">
-        <v>93.56398573966675</v>
+        <v>98.01614439340163</v>
       </c>
       <c r="F972" t="n">
-        <v>206.2711629616693</v>
+        <v>216.0863919296932</v>
       </c>
     </row>
     <row r="973" spans="1:6">
@@ -19987,16 +19987,16 @@
         <v>27</v>
       </c>
       <c r="C973" t="n">
-        <v>43986265264.57739</v>
+        <v>46425212773.755</v>
       </c>
       <c r="D973" t="n">
-        <v>105030331</v>
+        <v>106779623.23</v>
       </c>
       <c r="E973" t="n">
-        <v>418.7958358864679</v>
+        <v>434.7759560244611</v>
       </c>
       <c r="F973" t="n">
-        <v>923.2772997953072</v>
+        <v>958.507072651527</v>
       </c>
     </row>
     <row r="974" spans="1:6">
@@ -20007,16 +20007,16 @@
         <v>28</v>
       </c>
       <c r="C974" t="n">
-        <v>19764288224.18655</v>
+        <v>19087839522.89</v>
       </c>
       <c r="D974" t="n">
-        <v>56667037.27</v>
+        <v>56649885.13000001</v>
       </c>
       <c r="E974" t="n">
-        <v>348.7792758604293</v>
+        <v>336.9440110794096</v>
       </c>
       <c r="F974" t="n">
-        <v>768.9187915619024</v>
+        <v>742.8267668256664</v>
       </c>
     </row>
     <row r="975" spans="1:6">
@@ -20027,16 +20027,16 @@
         <v>29</v>
       </c>
       <c r="C975" t="n">
-        <v>52330770771.55927</v>
+        <v>53608179933.645</v>
       </c>
       <c r="D975" t="n">
-        <v>73791053.70000002</v>
+        <v>72928099.00999999</v>
       </c>
       <c r="E975" t="n">
-        <v>709.1750035757959</v>
+        <v>735.0826452543921</v>
       </c>
       <c r="F975" t="n">
-        <v>1563.4472128832</v>
+        <v>1620.563199727833</v>
       </c>
     </row>
     <row r="976" spans="1:6">
@@ -20047,16 +20047,16 @@
         <v>30</v>
       </c>
       <c r="C976" t="n">
-        <v>26512097215.38089</v>
+        <v>26401684013.88501</v>
       </c>
       <c r="D976" t="n">
-        <v>65781403.52999999</v>
+        <v>66596749.54</v>
       </c>
       <c r="E976" t="n">
-        <v>403.0333162972099</v>
+        <v>396.4410304744283</v>
       </c>
       <c r="F976" t="n">
-        <v>888.5272491088289</v>
+        <v>873.9938957839246</v>
       </c>
     </row>
     <row r="977" spans="1:6">
@@ -20067,16 +20067,16 @@
         <v>31</v>
       </c>
       <c r="C977" t="n">
-        <v>9723478626.075483</v>
+        <v>9946012778.515001</v>
       </c>
       <c r="D977" t="n">
-        <v>23664243.59</v>
+        <v>23387129.73</v>
       </c>
       <c r="E977" t="n">
-        <v>410.8932782531201</v>
+        <v>425.2771884938358</v>
       </c>
       <c r="F977" t="n">
-        <v>905.8553212368286</v>
+        <v>937.5660897535105</v>
       </c>
     </row>
     <row r="978" spans="1:6">
@@ -20087,16 +20087,16 @@
         <v>32</v>
       </c>
       <c r="C978" t="n">
-        <v>36767910527.61337</v>
+        <v>36996674429.12001</v>
       </c>
       <c r="D978" t="n">
-        <v>124312718.81</v>
+        <v>124723088.99</v>
       </c>
       <c r="E978" t="n">
-        <v>295.7694987253039</v>
+        <v>296.6305174825033</v>
       </c>
       <c r="F978" t="n">
-        <v>652.0534368898051</v>
+        <v>653.9516388419269</v>
       </c>
     </row>
     <row r="979" spans="1:6">
@@ -20107,16 +20107,16 @@
         <v>33</v>
       </c>
       <c r="C979" t="n">
-        <v>26830851576.61391</v>
+        <v>26309468763.495</v>
       </c>
       <c r="D979" t="n">
-        <v>42784985.48</v>
+        <v>42177239.91</v>
       </c>
       <c r="E979" t="n">
-        <v>627.1090494855044</v>
+        <v>623.7835576636953</v>
       </c>
       <c r="F979" t="n">
-        <v>1382.524610495743</v>
+        <v>1375.193231225383</v>
       </c>
     </row>
     <row r="980" spans="1:6">
@@ -20127,16 +20127,16 @@
         <v>34</v>
       </c>
       <c r="C980" t="n">
-        <v>20451669834.83244</v>
+        <v>20403141166.83</v>
       </c>
       <c r="D980" t="n">
-        <v>36748787.41</v>
+        <v>36869064.38</v>
       </c>
       <c r="E980" t="n">
-        <v>556.526385664284</v>
+        <v>553.394600864835</v>
       </c>
       <c r="F980" t="n">
-        <v>1226.918069835481</v>
+        <v>1220.013737066615</v>
       </c>
     </row>
     <row r="981" spans="1:6">
@@ -20147,16 +20147,16 @@
         <v>35</v>
       </c>
       <c r="C981" t="n">
-        <v>1673949742.494239</v>
+        <v>1703190526.915</v>
       </c>
       <c r="D981" t="n">
-        <v>16815626.76</v>
+        <v>16507489.16</v>
       </c>
       <c r="E981" t="n">
-        <v>99.54727030907524</v>
+        <v>103.1768375194256</v>
       </c>
       <c r="F981" t="n">
-        <v>219.4619121233873</v>
+        <v>227.4636559953258</v>
       </c>
     </row>
     <row r="982" spans="1:6">
@@ -20167,16 +20167,16 @@
         <v>36</v>
       </c>
       <c r="C982" t="n">
-        <v>13881727568.19452</v>
+        <v>13638395521.675</v>
       </c>
       <c r="D982" t="n">
-        <v>64001010.95</v>
+        <v>63610368.25</v>
       </c>
       <c r="E982" t="n">
-        <v>216.8985671029392</v>
+        <v>214.4052282180429</v>
       </c>
       <c r="F982" t="n">
-        <v>478.1745810351399</v>
+        <v>472.6777661294973</v>
       </c>
     </row>
     <row r="983" spans="1:6">
@@ -20187,16 +20187,16 @@
         <v>37</v>
       </c>
       <c r="C983" t="n">
-        <v>19779568388.30058</v>
+        <v>18646877069.49</v>
       </c>
       <c r="D983" t="n">
-        <v>34537197.22</v>
+        <v>34440788.78</v>
       </c>
       <c r="E983" t="n">
-        <v>572.7033453903583</v>
+        <v>541.4184091021274</v>
       </c>
       <c r="F983" t="n">
-        <v>1262.581795247584</v>
+        <v>1193.61102470655</v>
       </c>
     </row>
     <row r="984" spans="1:6">
@@ -20207,16 +20207,16 @@
         <v>38</v>
       </c>
       <c r="C984" t="n">
-        <v>13148226826.05747</v>
+        <v>13472639461.315</v>
       </c>
       <c r="D984" t="n">
-        <v>41490511.22000001</v>
+        <v>41404451.84</v>
       </c>
       <c r="E984" t="n">
-        <v>316.8971998522767</v>
+        <v>325.3910838713086</v>
       </c>
       <c r="F984" t="n">
-        <v>698.6315667943292</v>
+        <v>717.357183502687</v>
       </c>
     </row>
     <row r="985" spans="1:6">
@@ -20227,16 +20227,16 @@
         <v>39</v>
       </c>
       <c r="C985" t="n">
-        <v>25125058770.06453</v>
+        <v>24507030007.745</v>
       </c>
       <c r="D985" t="n">
-        <v>134281946.93</v>
+        <v>131720706.26</v>
       </c>
       <c r="E985" t="n">
-        <v>187.1067507172949</v>
+        <v>186.0529806101345</v>
       </c>
       <c r="F985" t="n">
-        <v>412.4955426313484</v>
+        <v>410.1724010531026</v>
       </c>
     </row>
     <row r="986" spans="1:6">
@@ -20247,16 +20247,16 @@
         <v>40</v>
       </c>
       <c r="C986" t="n">
-        <v>68056796722.34452</v>
+        <v>65933949834.02499</v>
       </c>
       <c r="D986" t="n">
-        <v>121189110.08</v>
+        <v>121377689.51</v>
       </c>
       <c r="E986" t="n">
-        <v>561.5751834254621</v>
+        <v>543.2130904798024</v>
       </c>
       <c r="F986" t="n">
-        <v>1238.048649379774</v>
+        <v>1197.567579271773</v>
       </c>
     </row>
     <row r="987" spans="1:6">
@@ -20267,16 +20267,16 @@
         <v>41</v>
       </c>
       <c r="C987" t="n">
-        <v>26517188419.56076</v>
+        <v>25163631641.95</v>
       </c>
       <c r="D987" t="n">
-        <v>83614322.06999999</v>
+        <v>82327506.45000002</v>
       </c>
       <c r="E987" t="n">
-        <v>317.1369182107484</v>
+        <v>305.6527851627893</v>
       </c>
       <c r="F987" t="n">
-        <v>699.1600498874159</v>
+        <v>673.8421301698852</v>
       </c>
     </row>
     <row r="988" spans="1:6">
@@ -20287,16 +20287,16 @@
         <v>42</v>
       </c>
       <c r="C988" t="n">
-        <v>9767671035.329494</v>
+        <v>9014398108.780001</v>
       </c>
       <c r="D988" t="n">
-        <v>65100775.36</v>
+        <v>63882109.08</v>
       </c>
       <c r="E988" t="n">
-        <v>150.0392427173927</v>
+        <v>141.1099013260694</v>
       </c>
       <c r="F988" t="n">
-        <v>330.7765144947639</v>
+        <v>311.0908884634526</v>
       </c>
     </row>
     <row r="989" spans="1:6">
@@ -20307,16 +20307,16 @@
         <v>43</v>
       </c>
       <c r="C989" t="n">
-        <v>72598815899.25462</v>
+        <v>71442693179.325</v>
       </c>
       <c r="D989" t="n">
-        <v>231406107.27</v>
+        <v>230732812.1500001</v>
       </c>
       <c r="E989" t="n">
-        <v>313.7290400661198</v>
+        <v>309.6338683415339</v>
       </c>
       <c r="F989" t="n">
-        <v>691.6470417297677</v>
+        <v>682.6188261457457</v>
       </c>
     </row>
     <row r="990" spans="1:6">
@@ -20327,16 +20327,16 @@
         <v>44</v>
       </c>
       <c r="C990" t="n">
-        <v>3197524198.504057</v>
+        <v>3279794938.465</v>
       </c>
       <c r="D990" t="n">
-        <v>8310605.739999999</v>
+        <v>9194153.629999999</v>
       </c>
       <c r="E990" t="n">
-        <v>384.7522429218327</v>
+        <v>356.7261403772084</v>
       </c>
       <c r="F990" t="n">
-        <v>848.2247947454724</v>
+        <v>786.4384490755938</v>
       </c>
     </row>
     <row r="991" spans="1:6">
@@ -20347,16 +20347,16 @@
         <v>45</v>
       </c>
       <c r="C991" t="n">
-        <v>22632517255.58004</v>
+        <v>22058289130.84499</v>
       </c>
       <c r="D991" t="n">
-        <v>98541994.52000001</v>
+        <v>98899721.37</v>
       </c>
       <c r="E991" t="n">
-        <v>229.6738295771612</v>
+        <v>223.0369188637179</v>
       </c>
       <c r="F991" t="n">
-        <v>506.3389246858096</v>
+        <v>491.7071913269524</v>
       </c>
     </row>
     <row r="992" spans="1:6">
@@ -20367,16 +20367,16 @@
         <v>46</v>
       </c>
       <c r="C992" t="n">
-        <v>2112685384.998585</v>
+        <v>2177994944.465</v>
       </c>
       <c r="D992" t="n">
-        <v>17014342.08</v>
+        <v>14148154.1</v>
       </c>
       <c r="E992" t="n">
-        <v>124.1708539222332</v>
+        <v>153.9419862881618</v>
       </c>
       <c r="F992" t="n">
-        <v>273.7470645569554</v>
+        <v>339.3805029708815</v>
       </c>
     </row>
     <row r="993" spans="1:6">
@@ -20387,16 +20387,16 @@
         <v>47</v>
       </c>
       <c r="C993" t="n">
-        <v>20934719722.75175</v>
+        <v>20182393107.71</v>
       </c>
       <c r="D993" t="n">
-        <v>77567623.92999999</v>
+        <v>80654750.28</v>
       </c>
       <c r="E993" t="n">
-        <v>269.8899187842088</v>
+        <v>250.231921091381</v>
       </c>
       <c r="F993" t="n">
-        <v>594.9993149516666</v>
+        <v>551.6612932380586</v>
       </c>
     </row>
     <row r="994" spans="1:6">
@@ -20407,16 +20407,16 @@
         <v>48</v>
       </c>
       <c r="C994" t="n">
-        <v>183315608049.2028</v>
+        <v>182046787955.734</v>
       </c>
       <c r="D994" t="n">
-        <v>477094719.6300001</v>
+        <v>475120529.48</v>
       </c>
       <c r="E994" t="n">
-        <v>384.2331522582539</v>
+        <v>383.1591704845437</v>
       </c>
       <c r="F994" t="n">
-        <v>847.0804074685467</v>
+        <v>844.712707250225</v>
       </c>
     </row>
     <row r="995" spans="1:6">
@@ -20427,16 +20427,16 @@
         <v>49</v>
       </c>
       <c r="C995" t="n">
-        <v>25774258851.83581</v>
+        <v>26164642569.955</v>
       </c>
       <c r="D995" t="n">
-        <v>37655318.6</v>
+        <v>37633458.85</v>
       </c>
       <c r="E995" t="n">
-        <v>684.4785759384282</v>
+        <v>695.2494766490219</v>
       </c>
       <c r="F995" t="n">
-        <v>1509.001468513859</v>
+        <v>1532.746996220434</v>
       </c>
     </row>
     <row r="996" spans="1:6">
@@ -20447,16 +20447,16 @@
         <v>50</v>
       </c>
       <c r="C996" t="n">
-        <v>29776091745.55735</v>
+        <v>30043610279.125</v>
       </c>
       <c r="D996" t="n">
-        <v>102478945.63</v>
+        <v>103269927.14</v>
       </c>
       <c r="E996" t="n">
-        <v>290.5581391622026</v>
+        <v>290.923128457288</v>
       </c>
       <c r="F996" t="n">
-        <v>640.5644735969919</v>
+        <v>641.3691289969372</v>
       </c>
     </row>
     <row r="997" spans="1:6">
@@ -20467,16 +20467,16 @@
         <v>51</v>
       </c>
       <c r="C997" t="n">
-        <v>1451738.276800026</v>
+        <v>3412102.735</v>
       </c>
       <c r="D997" t="n">
-        <v>2530918.75</v>
+        <v>2330291</v>
       </c>
       <c r="E997" t="n">
-        <v>0.5736012966832797</v>
+        <v>1.46423890192255</v>
       </c>
       <c r="F997" t="n">
-        <v>1.264561418667959</v>
+        <v>3.228061083178453</v>
       </c>
     </row>
     <row r="998" spans="1:6">
@@ -20487,16 +20487,16 @@
         <v>52</v>
       </c>
       <c r="C998" t="n">
-        <v>11482373688.1693</v>
+        <v>11174172620.94</v>
       </c>
       <c r="D998" t="n">
-        <v>114442526.99</v>
+        <v>116364402.01</v>
       </c>
       <c r="E998" t="n">
-        <v>100.3331016028039</v>
+        <v>96.0274141225744</v>
       </c>
       <c r="F998" t="n">
-        <v>221.1943557935415</v>
+        <v>211.7020371746275</v>
       </c>
     </row>
     <row r="999" spans="1:6">
@@ -20507,16 +20507,16 @@
         <v>53</v>
       </c>
       <c r="C999" t="n">
-        <v>32404283369.72654</v>
+        <v>31329690492.265</v>
       </c>
       <c r="D999" t="n">
-        <v>61042861.09999999</v>
+        <v>61578043.54000001</v>
       </c>
       <c r="E999" t="n">
-        <v>530.8447668703154</v>
+        <v>508.780219233724</v>
       </c>
       <c r="F999" t="n">
-        <v>1170.300373042297</v>
+        <v>1121.656871322668</v>
       </c>
     </row>
     <row r="1000" spans="1:6">
@@ -20527,16 +20527,16 @@
         <v>54</v>
       </c>
       <c r="C1000" t="n">
-        <v>48897052155.93681</v>
+        <v>49285391158.88</v>
       </c>
       <c r="D1000" t="n">
-        <v>56773422.83000001</v>
+        <v>56676905.86</v>
       </c>
       <c r="E1000" t="n">
-        <v>861.2665877544873</v>
+        <v>869.5850701628262</v>
       </c>
       <c r="F1000" t="n">
-        <v>1898.748319363543</v>
+        <v>1917.087245680967</v>
       </c>
     </row>
     <row r="1001" spans="1:6">
@@ -20547,16 +20547,16 @@
         <v>55</v>
       </c>
       <c r="C1001" t="n">
-        <v>37169259410.77391</v>
+        <v>35642422641.785</v>
       </c>
       <c r="D1001" t="n">
-        <v>41663480.84</v>
+        <v>42023950.27999999</v>
       </c>
       <c r="E1001" t="n">
-        <v>892.1304380091231</v>
+        <v>848.1454600127851</v>
       </c>
       <c r="F1001" t="n">
-        <v>1966.790763634913</v>
+        <v>1869.821481144186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022 Q2 update, includes cems_new.py, which provides a manual fix to accessing the EPA ftp site. this script needs to be incorporated into the cems.py file in order to automate it instead of it being a manual fix.
</commit_message>
<xml_diff>
--- a/web_files/US State Power Sector CO2 Emissions.xlsx
+++ b/web_files/US State Power Sector CO2 Emissions.xlsx
@@ -987,13 +987,13 @@
         <v>27</v>
       </c>
       <c r="C23" t="n">
-        <v>75251889187.105</v>
+        <v>75251889187.10501</v>
       </c>
       <c r="D23" t="n">
         <v>111845612</v>
       </c>
       <c r="E23" t="n">
-        <v>672.81932515247</v>
+        <v>672.8193251524701</v>
       </c>
       <c r="F23" t="n">
         <v>1483.297484231136</v>
@@ -1733,7 +1733,7 @@
         <v>203352778</v>
       </c>
       <c r="E60" t="n">
-        <v>607.0440914077899</v>
+        <v>607.0440914077898</v>
       </c>
       <c r="F60" t="n">
         <v>1338.289403917614</v>
@@ -2173,10 +2173,10 @@
         <v>61569386</v>
       </c>
       <c r="E82" t="n">
-        <v>334.0726153689433</v>
+        <v>334.0726153689432</v>
       </c>
       <c r="F82" t="n">
-        <v>736.4964878423724</v>
+        <v>736.4964878423723</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3907,13 +3907,13 @@
         <v>23</v>
       </c>
       <c r="C169" t="n">
-        <v>50732697297.78251</v>
+        <v>50732697297.7825</v>
       </c>
       <c r="D169" t="n">
         <v>98172308.65000001</v>
       </c>
       <c r="E169" t="n">
-        <v>516.7719695647853</v>
+        <v>516.7719695647852</v>
       </c>
       <c r="F169" t="n">
         <v>1139.275484102526</v>
@@ -6027,13 +6027,13 @@
         <v>29</v>
       </c>
       <c r="C275" t="n">
-        <v>79695807549.96605</v>
+        <v>79695807549.96606</v>
       </c>
       <c r="D275" t="n">
         <v>91686342.91</v>
       </c>
       <c r="E275" t="n">
-        <v>869.2222311472937</v>
+        <v>869.2222311472939</v>
       </c>
       <c r="F275" t="n">
         <v>1916.287330787324</v>
@@ -6053,7 +6053,7 @@
         <v>46228847.42</v>
       </c>
       <c r="E276" t="n">
-        <v>554.9665658524307</v>
+        <v>554.9665658524308</v>
       </c>
       <c r="F276" t="n">
         <v>1223.479291078269</v>
@@ -7907,16 +7907,16 @@
         <v>23</v>
       </c>
       <c r="C369" t="n">
-        <v>49337093172.35</v>
+        <v>49337093172.35001</v>
       </c>
       <c r="D369" t="n">
         <v>92453141.40999997</v>
       </c>
       <c r="E369" t="n">
-        <v>533.6443134317724</v>
+        <v>533.6443134317725</v>
       </c>
       <c r="F369" t="n">
-        <v>1176.472253391685</v>
+        <v>1176.472253391686</v>
       </c>
     </row>
     <row r="370" spans="1:6">
@@ -7927,13 +7927,13 @@
         <v>24</v>
       </c>
       <c r="C370" t="n">
-        <v>21611840237.56501</v>
+        <v>21611840237.565</v>
       </c>
       <c r="D370" t="n">
         <v>42505478.51</v>
       </c>
       <c r="E370" t="n">
-        <v>508.4483458404197</v>
+        <v>508.4483458404196</v>
       </c>
       <c r="F370" t="n">
         <v>1120.925223239789</v>
@@ -10733,10 +10733,10 @@
         <v>221923641.13</v>
       </c>
       <c r="E510" t="n">
-        <v>504.7993257629822</v>
+        <v>504.7993257629821</v>
       </c>
       <c r="F510" t="n">
-        <v>1112.880593577071</v>
+        <v>1112.88059357707</v>
       </c>
     </row>
     <row r="511" spans="1:6">
@@ -11113,7 +11113,7 @@
         <v>35079900.14000001</v>
       </c>
       <c r="E529" t="n">
-        <v>841.6477784246621</v>
+        <v>841.6477784246622</v>
       </c>
       <c r="F529" t="n">
         <v>1855.49669231501</v>
@@ -14250,13 +14250,13 @@
         <v>96841012206.02176</v>
       </c>
       <c r="D686" t="n">
-        <v>134559118.48</v>
+        <v>134585276.5</v>
       </c>
       <c r="E686" t="n">
-        <v>719.6911907565418</v>
+        <v>719.5513114394929</v>
       </c>
       <c r="F686" t="n">
-        <v>1586.631199141872</v>
+        <v>1586.322821199506</v>
       </c>
     </row>
     <row r="687" spans="1:6">
@@ -15250,13 +15250,13 @@
         <v>81804797679.51239</v>
       </c>
       <c r="D736" t="n">
-        <v>121988463.49</v>
+        <v>123174356.23</v>
       </c>
       <c r="E736" t="n">
-        <v>670.5945409847575</v>
+        <v>664.1382198642111</v>
       </c>
       <c r="F736" t="n">
-        <v>1478.392725054996</v>
+        <v>1464.15911951264</v>
       </c>
     </row>
     <row r="737" spans="1:6">
@@ -16250,13 +16250,13 @@
         <v>79037983158.18074</v>
       </c>
       <c r="D786" t="n">
-        <v>119029994.13</v>
+        <v>119993982.13</v>
       </c>
       <c r="E786" t="n">
-        <v>664.0173658402308</v>
+        <v>658.682891884961</v>
       </c>
       <c r="F786" t="n">
-        <v>1463.892684731373</v>
+        <v>1452.132303449585</v>
       </c>
     </row>
     <row r="787" spans="1:6">
@@ -16310,13 +16310,13 @@
         <v>83808466141.26736</v>
       </c>
       <c r="D789" t="n">
-        <v>215328245.01</v>
+        <v>215328244.99</v>
       </c>
       <c r="E789" t="n">
-        <v>389.2126002205388</v>
+        <v>389.2126002566894</v>
       </c>
       <c r="F789" t="n">
-        <v>858.0580984461998</v>
+        <v>858.0580985258975</v>
       </c>
     </row>
     <row r="790" spans="1:6">
@@ -17250,13 +17250,13 @@
         <v>78271359245.65692</v>
       </c>
       <c r="D836" t="n">
-        <v>119683315.56</v>
+        <v>120943352.56</v>
       </c>
       <c r="E836" t="n">
-        <v>653.9872235275576</v>
+        <v>647.1737188435098</v>
       </c>
       <c r="F836" t="n">
-        <v>1441.780232988854</v>
+        <v>1426.759180562402</v>
       </c>
     </row>
     <row r="837" spans="1:6">
@@ -18250,13 +18250,13 @@
         <v>75497054015.65343</v>
       </c>
       <c r="D886" t="n">
-        <v>126337574.67</v>
+        <v>128090252.67</v>
       </c>
       <c r="E886" t="n">
-        <v>597.581948306792</v>
+        <v>589.4051455277953</v>
       </c>
       <c r="F886" t="n">
-        <v>1317.429163237154</v>
+        <v>1299.402583830578</v>
       </c>
     </row>
     <row r="887" spans="1:6">
@@ -18267,16 +18267,16 @@
         <v>41</v>
       </c>
       <c r="C887" t="n">
-        <v>34615865006.30135</v>
+        <v>34624998004.3531</v>
       </c>
       <c r="D887" t="n">
-        <v>86234853.75999998</v>
+        <v>87192534.75999998</v>
       </c>
       <c r="E887" t="n">
-        <v>401.4138541086958</v>
+        <v>397.1096619642889</v>
       </c>
       <c r="F887" t="n">
-        <v>884.9569827680308</v>
+        <v>875.4679607664713</v>
       </c>
     </row>
     <row r="888" spans="1:6">
@@ -19250,13 +19250,13 @@
         <v>66724266888.81259</v>
       </c>
       <c r="D936" t="n">
-        <v>120195276.17</v>
+        <v>121744273.17</v>
       </c>
       <c r="E936" t="n">
-        <v>555.1321900075351</v>
+        <v>548.0690397292107</v>
       </c>
       <c r="F936" t="n">
-        <v>1223.844426090612</v>
+        <v>1208.273004987018</v>
       </c>
     </row>
     <row r="937" spans="1:6">
@@ -19267,16 +19267,16 @@
         <v>41</v>
       </c>
       <c r="C937" t="n">
-        <v>28394302215.716</v>
+        <v>28463920889.54651</v>
       </c>
       <c r="D937" t="n">
-        <v>85236019.98999998</v>
+        <v>86405688.98999999</v>
       </c>
       <c r="E937" t="n">
-        <v>333.1256224662679</v>
+        <v>329.4218381018954</v>
       </c>
       <c r="F937" t="n">
-        <v>734.4087472891342</v>
+        <v>726.2433842794387</v>
       </c>
     </row>
     <row r="938" spans="1:6">
@@ -19587,16 +19587,16 @@
         <v>7</v>
       </c>
       <c r="C953" t="n">
-        <v>42560364927.26501</v>
+        <v>44587025850.98647</v>
       </c>
       <c r="D953" t="n">
-        <v>137542701.67</v>
+        <v>137547376.55</v>
       </c>
       <c r="E953" t="n">
-        <v>309.43382971623</v>
+        <v>324.1575882385412</v>
       </c>
       <c r="F953" t="n">
-        <v>682.1778209924008</v>
+        <v>714.6378190306879</v>
       </c>
     </row>
     <row r="954" spans="1:6">
@@ -19607,16 +19607,16 @@
         <v>8</v>
       </c>
       <c r="C954" t="n">
-        <v>22605591632.085</v>
+        <v>23437284105.957</v>
       </c>
       <c r="D954" t="n">
         <v>54727500.27999999</v>
       </c>
       <c r="E954" t="n">
-        <v>413.0572658431131</v>
+        <v>428.2542412141212</v>
       </c>
       <c r="F954" t="n">
-        <v>910.6260482777271</v>
+        <v>944.1293001806516</v>
       </c>
     </row>
     <row r="955" spans="1:6">
@@ -19627,16 +19627,16 @@
         <v>9</v>
       </c>
       <c r="C955" t="n">
-        <v>35708721850.66</v>
+        <v>40072667006.29189</v>
       </c>
       <c r="D955" t="n">
         <v>112992809.25</v>
       </c>
       <c r="E955" t="n">
-        <v>316.0264983911798</v>
+        <v>354.6479397430496</v>
       </c>
       <c r="F955" t="n">
-        <v>696.7120183531949</v>
+        <v>781.8568479575271</v>
       </c>
     </row>
     <row r="956" spans="1:6">
@@ -19647,16 +19647,16 @@
         <v>10</v>
       </c>
       <c r="C956" t="n">
-        <v>37774782667.21999</v>
+        <v>39106013752.5272</v>
       </c>
       <c r="D956" t="n">
-        <v>212702187.88</v>
+        <v>212710794.88</v>
       </c>
       <c r="E956" t="n">
-        <v>177.5947066822433</v>
+        <v>183.8459292796528</v>
       </c>
       <c r="F956" t="n">
-        <v>391.5252903516736</v>
+        <v>405.3067356899224</v>
       </c>
     </row>
     <row r="957" spans="1:6">
@@ -19667,16 +19667,16 @@
         <v>11</v>
       </c>
       <c r="C957" t="n">
-        <v>28892082200.82</v>
+        <v>29557881812.20951</v>
       </c>
       <c r="D957" t="n">
         <v>54815696.35</v>
       </c>
       <c r="E957" t="n">
-        <v>527.0768069120771</v>
+        <v>539.222955838807</v>
       </c>
       <c r="F957" t="n">
-        <v>1161.993528518365</v>
+        <v>1188.770928442234</v>
       </c>
     </row>
     <row r="958" spans="1:6">
@@ -19687,16 +19687,16 @@
         <v>12</v>
       </c>
       <c r="C958" t="n">
-        <v>9972877697.759998</v>
+        <v>9951530131.34798</v>
       </c>
       <c r="D958" t="n">
         <v>41925724.74</v>
       </c>
       <c r="E958" t="n">
-        <v>237.8701324689372</v>
+        <v>237.3609566217836</v>
       </c>
       <c r="F958" t="n">
-        <v>524.408494041019</v>
+        <v>523.2859649683842</v>
       </c>
     </row>
     <row r="959" spans="1:6">
@@ -19707,16 +19707,16 @@
         <v>13</v>
       </c>
       <c r="C959" t="n">
-        <v>2079263866.375</v>
+        <v>1774201621.423324</v>
       </c>
       <c r="D959" t="n">
         <v>5333805.300000001</v>
       </c>
       <c r="E959" t="n">
-        <v>389.8274776499621</v>
+        <v>332.63336804276</v>
       </c>
       <c r="F959" t="n">
-        <v>859.4136572271066</v>
+        <v>733.3235231870686</v>
       </c>
     </row>
     <row r="960" spans="1:6">
@@ -19727,16 +19727,16 @@
         <v>14</v>
       </c>
       <c r="C960" t="n">
-        <v>95440192441.855</v>
+        <v>95279631022.79845</v>
       </c>
       <c r="D960" t="n">
         <v>251974893.25</v>
       </c>
       <c r="E960" t="n">
-        <v>378.7686590947885</v>
+        <v>378.1314471210653</v>
       </c>
       <c r="F960" t="n">
-        <v>835.0333858403708</v>
+        <v>833.6285883231005</v>
       </c>
     </row>
     <row r="961" spans="1:6">
@@ -19747,16 +19747,16 @@
         <v>15</v>
       </c>
       <c r="C961" t="n">
-        <v>37730463955.495</v>
+        <v>38843590090.62013</v>
       </c>
       <c r="D961" t="n">
-        <v>120326774.35</v>
+        <v>120329712.2</v>
       </c>
       <c r="E961" t="n">
-        <v>313.5666534677201</v>
+        <v>322.8096318061345</v>
       </c>
       <c r="F961" t="n">
-        <v>691.2890442349359</v>
+        <v>711.6661142798041</v>
       </c>
     </row>
     <row r="962" spans="1:6">
@@ -19767,16 +19767,16 @@
         <v>16</v>
       </c>
       <c r="C962" t="n">
-        <v>6535712231.1</v>
+        <v>6535711791.630001</v>
       </c>
       <c r="D962" t="n">
         <v>10289725.16</v>
       </c>
       <c r="E962" t="n">
-        <v>635.1687853147674</v>
+        <v>635.168742605172</v>
       </c>
       <c r="F962" t="n">
-        <v>1400.293104104936</v>
+        <v>1400.293009947362</v>
       </c>
     </row>
     <row r="963" spans="1:6">
@@ -19787,16 +19787,16 @@
         <v>17</v>
       </c>
       <c r="C963" t="n">
-        <v>16296664463.41</v>
+        <v>16713488679.01489</v>
       </c>
       <c r="D963" t="n">
         <v>59846494.78</v>
       </c>
       <c r="E963" t="n">
-        <v>272.3077520800125</v>
+        <v>279.2726414546896</v>
       </c>
       <c r="F963" t="n">
-        <v>600.3296702355956</v>
+        <v>615.6844653510086</v>
       </c>
     </row>
     <row r="964" spans="1:6">
@@ -19807,16 +19807,16 @@
         <v>18</v>
       </c>
       <c r="C964" t="n">
-        <v>1708644232.975</v>
+        <v>1701863321.565638</v>
       </c>
       <c r="D964" t="n">
         <v>17773269.45</v>
       </c>
       <c r="E964" t="n">
-        <v>96.13561746654327</v>
+        <v>95.7540944480329</v>
       </c>
       <c r="F964" t="n">
-        <v>211.9405822667413</v>
+        <v>211.0994766201333</v>
       </c>
     </row>
     <row r="965" spans="1:6">
@@ -19827,16 +19827,16 @@
         <v>19</v>
       </c>
       <c r="C965" t="n">
-        <v>43331370870.71499</v>
+        <v>43478998413.15931</v>
       </c>
       <c r="D965" t="n">
         <v>173821585.18</v>
       </c>
       <c r="E965" t="n">
-        <v>249.2864785799958</v>
+        <v>250.1357835859963</v>
       </c>
       <c r="F965" t="n">
-        <v>549.5769706774588</v>
+        <v>551.4493484936876</v>
       </c>
     </row>
     <row r="966" spans="1:6">
@@ -19847,16 +19847,16 @@
         <v>20</v>
       </c>
       <c r="C966" t="n">
-        <v>63967371194.355</v>
+        <v>63985081277.39812</v>
       </c>
       <c r="D966" t="n">
         <v>90240205.28999998</v>
       </c>
       <c r="E966" t="n">
-        <v>708.8566674775016</v>
+        <v>709.0529223839063</v>
       </c>
       <c r="F966" t="n">
-        <v>1562.7454091209</v>
+        <v>1563.17807268756</v>
       </c>
     </row>
     <row r="967" spans="1:6">
@@ -19867,16 +19867,16 @@
         <v>21</v>
       </c>
       <c r="C967" t="n">
-        <v>20157001750.585</v>
+        <v>19737749112.21638</v>
       </c>
       <c r="D967" t="n">
         <v>54589706.59999999</v>
       </c>
       <c r="E967" t="n">
-        <v>369.2454678000596</v>
+        <v>361.5654001741124</v>
       </c>
       <c r="F967" t="n">
-        <v>814.0385583120114</v>
+        <v>797.1070812238481</v>
       </c>
     </row>
     <row r="968" spans="1:6">
@@ -19887,16 +19887,16 @@
         <v>22</v>
       </c>
       <c r="C968" t="n">
-        <v>49247599870.59</v>
+        <v>48418067110.35614</v>
       </c>
       <c r="D968" t="n">
         <v>63590731.15000001</v>
       </c>
       <c r="E968" t="n">
-        <v>774.446196481419</v>
+        <v>761.4013274378924</v>
       </c>
       <c r="F968" t="n">
-        <v>1707.344084762936</v>
+        <v>1678.585366469578</v>
       </c>
     </row>
     <row r="969" spans="1:6">
@@ -19907,16 +19907,16 @@
         <v>23</v>
       </c>
       <c r="C969" t="n">
-        <v>36052740045.305</v>
+        <v>35434304739.98317</v>
       </c>
       <c r="D969" t="n">
-        <v>101030769.69</v>
+        <v>101030770.46</v>
       </c>
       <c r="E969" t="n">
-        <v>356.8491080086613</v>
+        <v>350.7278483441071</v>
       </c>
       <c r="F969" t="n">
-        <v>786.7095435158949</v>
+        <v>773.2146144594185</v>
       </c>
     </row>
     <row r="970" spans="1:6">
@@ -19927,16 +19927,16 @@
         <v>24</v>
       </c>
       <c r="C970" t="n">
-        <v>7183269475.57</v>
+        <v>7133516031.947849</v>
       </c>
       <c r="D970" t="n">
         <v>20535999.84</v>
       </c>
       <c r="E970" t="n">
-        <v>349.7891279478116</v>
+        <v>347.3663852515811</v>
       </c>
       <c r="F970" t="n">
-        <v>771.1451114737455</v>
+        <v>765.8039329256358</v>
       </c>
     </row>
     <row r="971" spans="1:6">
@@ -19947,16 +19947,16 @@
         <v>25</v>
       </c>
       <c r="C971" t="n">
-        <v>9777720690.965</v>
+        <v>10572680075.41615</v>
       </c>
       <c r="D971" t="n">
         <v>37023543.94</v>
       </c>
       <c r="E971" t="n">
-        <v>264.094671942013</v>
+        <v>285.566397764356</v>
       </c>
       <c r="F971" t="n">
-        <v>582.2231137633618</v>
+        <v>629.5596805112992</v>
       </c>
     </row>
     <row r="972" spans="1:6">
@@ -19967,16 +19967,16 @@
         <v>26</v>
       </c>
       <c r="C972" t="n">
-        <v>989074059.7849998</v>
+        <v>972318018.7311822</v>
       </c>
       <c r="D972" t="n">
         <v>10090930.08</v>
       </c>
       <c r="E972" t="n">
-        <v>98.01614439340163</v>
+        <v>96.35563927435143</v>
       </c>
       <c r="F972" t="n">
-        <v>216.0863919296932</v>
+        <v>212.4256423442352</v>
       </c>
     </row>
     <row r="973" spans="1:6">
@@ -19987,16 +19987,16 @@
         <v>27</v>
       </c>
       <c r="C973" t="n">
-        <v>46425212773.755</v>
+        <v>45084303268.95815</v>
       </c>
       <c r="D973" t="n">
         <v>106779623.23</v>
       </c>
       <c r="E973" t="n">
-        <v>434.7759560244611</v>
+        <v>422.2182276467483</v>
       </c>
       <c r="F973" t="n">
-        <v>958.507072651527</v>
+        <v>930.8223046700215</v>
       </c>
     </row>
     <row r="974" spans="1:6">
@@ -20007,16 +20007,16 @@
         <v>28</v>
       </c>
       <c r="C974" t="n">
-        <v>19087839522.89</v>
+        <v>19796961317.84272</v>
       </c>
       <c r="D974" t="n">
         <v>56649885.13000001</v>
       </c>
       <c r="E974" t="n">
-        <v>336.9440110794096</v>
+        <v>349.4616321359294</v>
       </c>
       <c r="F974" t="n">
-        <v>742.8267668256664</v>
+        <v>770.42311420687</v>
       </c>
     </row>
     <row r="975" spans="1:6">
@@ -20027,16 +20027,16 @@
         <v>29</v>
       </c>
       <c r="C975" t="n">
-        <v>53608179933.645</v>
+        <v>52212007528.87102</v>
       </c>
       <c r="D975" t="n">
         <v>72928099.00999999</v>
       </c>
       <c r="E975" t="n">
-        <v>735.0826452543921</v>
+        <v>715.9381395874811</v>
       </c>
       <c r="F975" t="n">
-        <v>1620.563199727833</v>
+        <v>1578.357222534561</v>
       </c>
     </row>
     <row r="976" spans="1:6">
@@ -20047,16 +20047,16 @@
         <v>30</v>
       </c>
       <c r="C976" t="n">
-        <v>26401684013.88501</v>
+        <v>26875063169.98458</v>
       </c>
       <c r="D976" t="n">
-        <v>66596749.54</v>
+        <v>66596727.12</v>
       </c>
       <c r="E976" t="n">
-        <v>396.4410304744283</v>
+        <v>403.5493083850602</v>
       </c>
       <c r="F976" t="n">
-        <v>873.9938957839246</v>
+        <v>889.6648052657038</v>
       </c>
     </row>
     <row r="977" spans="1:6">
@@ -20067,16 +20067,16 @@
         <v>31</v>
       </c>
       <c r="C977" t="n">
-        <v>9946012778.515001</v>
+        <v>9696593641.873693</v>
       </c>
       <c r="D977" t="n">
         <v>23387129.73</v>
       </c>
       <c r="E977" t="n">
-        <v>425.2771884938358</v>
+        <v>414.6123852657012</v>
       </c>
       <c r="F977" t="n">
-        <v>937.5660897535105</v>
+        <v>914.0544645567649</v>
       </c>
     </row>
     <row r="978" spans="1:6">
@@ -20087,16 +20087,16 @@
         <v>32</v>
       </c>
       <c r="C978" t="n">
-        <v>36996674429.12001</v>
+        <v>36550083393.9627</v>
       </c>
       <c r="D978" t="n">
         <v>124723088.99</v>
       </c>
       <c r="E978" t="n">
-        <v>296.6305174825033</v>
+        <v>293.0498570067744</v>
       </c>
       <c r="F978" t="n">
-        <v>653.9516388419269</v>
+        <v>646.0577147571349</v>
       </c>
     </row>
     <row r="979" spans="1:6">
@@ -20107,16 +20107,16 @@
         <v>33</v>
       </c>
       <c r="C979" t="n">
-        <v>26309468763.495</v>
+        <v>26719962124.51554</v>
       </c>
       <c r="D979" t="n">
         <v>42177239.91</v>
       </c>
       <c r="E979" t="n">
-        <v>623.7835576636953</v>
+        <v>633.5161376498792</v>
       </c>
       <c r="F979" t="n">
-        <v>1375.193231225383</v>
+        <v>1396.649677062924</v>
       </c>
     </row>
     <row r="980" spans="1:6">
@@ -20127,16 +20127,16 @@
         <v>34</v>
       </c>
       <c r="C980" t="n">
-        <v>20403141166.83</v>
+        <v>20140759295.87116</v>
       </c>
       <c r="D980" t="n">
         <v>36869064.38</v>
       </c>
       <c r="E980" t="n">
-        <v>553.394600864835</v>
+        <v>546.2780147683033</v>
       </c>
       <c r="F980" t="n">
-        <v>1220.013737066615</v>
+        <v>1204.324511358201</v>
       </c>
     </row>
     <row r="981" spans="1:6">
@@ -20147,16 +20147,16 @@
         <v>35</v>
       </c>
       <c r="C981" t="n">
-        <v>1703190526.915</v>
+        <v>1675341978.376426</v>
       </c>
       <c r="D981" t="n">
         <v>16507489.16</v>
       </c>
       <c r="E981" t="n">
-        <v>103.1768375194256</v>
+        <v>101.4898124201722</v>
       </c>
       <c r="F981" t="n">
-        <v>227.4636559953258</v>
+        <v>223.7444404615116</v>
       </c>
     </row>
     <row r="982" spans="1:6">
@@ -20167,16 +20167,16 @@
         <v>36</v>
       </c>
       <c r="C982" t="n">
-        <v>13638395521.675</v>
+        <v>13732939819.6346</v>
       </c>
       <c r="D982" t="n">
         <v>63610368.25</v>
       </c>
       <c r="E982" t="n">
-        <v>214.4052282180429</v>
+        <v>215.8915314821276</v>
       </c>
       <c r="F982" t="n">
-        <v>472.6777661294973</v>
+        <v>475.9544703054985</v>
       </c>
     </row>
     <row r="983" spans="1:6">
@@ -20187,16 +20187,16 @@
         <v>37</v>
       </c>
       <c r="C983" t="n">
-        <v>18646877069.49</v>
+        <v>19329404742.66918</v>
       </c>
       <c r="D983" t="n">
         <v>34440788.78</v>
       </c>
       <c r="E983" t="n">
-        <v>541.4184091021274</v>
+        <v>561.2358319125924</v>
       </c>
       <c r="F983" t="n">
-        <v>1193.61102470655</v>
+        <v>1237.300515034501</v>
       </c>
     </row>
     <row r="984" spans="1:6">
@@ -20207,16 +20207,16 @@
         <v>38</v>
       </c>
       <c r="C984" t="n">
-        <v>13472639461.315</v>
+        <v>13343373492.75728</v>
       </c>
       <c r="D984" t="n">
         <v>41404451.84</v>
       </c>
       <c r="E984" t="n">
-        <v>325.3910838713086</v>
+        <v>322.269053200374</v>
       </c>
       <c r="F984" t="n">
-        <v>717.357183502687</v>
+        <v>710.4743546855445</v>
       </c>
     </row>
     <row r="985" spans="1:6">
@@ -20227,16 +20227,16 @@
         <v>39</v>
       </c>
       <c r="C985" t="n">
-        <v>24507030007.745</v>
+        <v>25662350760.38052</v>
       </c>
       <c r="D985" t="n">
         <v>131720706.26</v>
       </c>
       <c r="E985" t="n">
-        <v>186.0529806101345</v>
+        <v>194.823968751931</v>
       </c>
       <c r="F985" t="n">
-        <v>410.1724010531026</v>
+        <v>429.5089215105072</v>
       </c>
     </row>
     <row r="986" spans="1:6">
@@ -20247,16 +20247,16 @@
         <v>40</v>
       </c>
       <c r="C986" t="n">
-        <v>65933949834.02499</v>
+        <v>68025530179.3708</v>
       </c>
       <c r="D986" t="n">
-        <v>121377689.51</v>
+        <v>122923138.51</v>
       </c>
       <c r="E986" t="n">
-        <v>543.2130904798024</v>
+        <v>553.3989044205604</v>
       </c>
       <c r="F986" t="n">
-        <v>1197.567579271773</v>
+        <v>1220.023224685567</v>
       </c>
     </row>
     <row r="987" spans="1:6">
@@ -20267,16 +20267,16 @@
         <v>41</v>
       </c>
       <c r="C987" t="n">
-        <v>25163631641.95</v>
+        <v>26419863688.18068</v>
       </c>
       <c r="D987" t="n">
-        <v>82327506.45000002</v>
+        <v>83397403.44999999</v>
       </c>
       <c r="E987" t="n">
-        <v>305.6527851627893</v>
+        <v>316.7947993011608</v>
       </c>
       <c r="F987" t="n">
-        <v>673.8421301698852</v>
+        <v>698.4058145393392</v>
       </c>
     </row>
     <row r="988" spans="1:6">
@@ -20287,16 +20287,16 @@
         <v>42</v>
       </c>
       <c r="C988" t="n">
-        <v>9014398108.780001</v>
+        <v>9861669212.132658</v>
       </c>
       <c r="D988" t="n">
         <v>63882109.08</v>
       </c>
       <c r="E988" t="n">
-        <v>141.1099013260694</v>
+        <v>154.3729434446634</v>
       </c>
       <c r="F988" t="n">
-        <v>311.0908884634526</v>
+        <v>340.330591118105</v>
       </c>
     </row>
     <row r="989" spans="1:6">
@@ -20307,16 +20307,16 @@
         <v>43</v>
       </c>
       <c r="C989" t="n">
-        <v>71442693179.325</v>
+        <v>73047922783.51036</v>
       </c>
       <c r="D989" t="n">
         <v>230732812.1500001</v>
       </c>
       <c r="E989" t="n">
-        <v>309.6338683415339</v>
+        <v>316.5909612197752</v>
       </c>
       <c r="F989" t="n">
-        <v>682.6188261457457</v>
+        <v>697.9564331051165</v>
       </c>
     </row>
     <row r="990" spans="1:6">
@@ -20327,16 +20327,16 @@
         <v>44</v>
       </c>
       <c r="C990" t="n">
-        <v>3279794938.465</v>
+        <v>3336839504.475111</v>
       </c>
       <c r="D990" t="n">
         <v>9194153.629999999</v>
       </c>
       <c r="E990" t="n">
-        <v>356.7261403772084</v>
+        <v>362.9305794485742</v>
       </c>
       <c r="F990" t="n">
-        <v>786.4384490755938</v>
+        <v>800.1167554523266</v>
       </c>
     </row>
     <row r="991" spans="1:6">
@@ -20347,16 +20347,16 @@
         <v>45</v>
       </c>
       <c r="C991" t="n">
-        <v>22058289130.84499</v>
+        <v>22613927867.88196</v>
       </c>
       <c r="D991" t="n">
         <v>98899721.37</v>
       </c>
       <c r="E991" t="n">
-        <v>223.0369188637179</v>
+        <v>228.6551221239498</v>
       </c>
       <c r="F991" t="n">
-        <v>491.7071913269524</v>
+        <v>504.0930822344597</v>
       </c>
     </row>
     <row r="992" spans="1:6">
@@ -20367,16 +20367,16 @@
         <v>46</v>
       </c>
       <c r="C992" t="n">
-        <v>2177994944.465</v>
+        <v>2283062536.290447</v>
       </c>
       <c r="D992" t="n">
         <v>14148154.1</v>
       </c>
       <c r="E992" t="n">
-        <v>153.9419862881618</v>
+        <v>161.3682265653615</v>
       </c>
       <c r="F992" t="n">
-        <v>339.3805029708815</v>
+        <v>355.7523922859959</v>
       </c>
     </row>
     <row r="993" spans="1:6">
@@ -20387,16 +20387,16 @@
         <v>47</v>
       </c>
       <c r="C993" t="n">
-        <v>20182393107.71</v>
+        <v>20697758452.77121</v>
       </c>
       <c r="D993" t="n">
         <v>80654750.28</v>
       </c>
       <c r="E993" t="n">
-        <v>250.231921091381</v>
+        <v>256.6216916042408</v>
       </c>
       <c r="F993" t="n">
-        <v>551.6612932380586</v>
+        <v>565.7481813107092</v>
       </c>
     </row>
     <row r="994" spans="1:6">
@@ -20407,16 +20407,16 @@
         <v>48</v>
       </c>
       <c r="C994" t="n">
-        <v>182046787955.734</v>
+        <v>182562331365.7779</v>
       </c>
       <c r="D994" t="n">
-        <v>475120529.48</v>
+        <v>475120546.72</v>
       </c>
       <c r="E994" t="n">
-        <v>383.1591704845437</v>
+        <v>384.2442357546921</v>
       </c>
       <c r="F994" t="n">
-        <v>844.712707250225</v>
+        <v>847.1048421447942</v>
       </c>
     </row>
     <row r="995" spans="1:6">
@@ -20427,16 +20427,16 @@
         <v>49</v>
       </c>
       <c r="C995" t="n">
-        <v>26164642569.955</v>
+        <v>25833489925.8673</v>
       </c>
       <c r="D995" t="n">
         <v>37633458.85</v>
       </c>
       <c r="E995" t="n">
-        <v>695.2494766490219</v>
+        <v>686.4500557558317</v>
       </c>
       <c r="F995" t="n">
-        <v>1532.746996220434</v>
+        <v>1513.347792919307</v>
       </c>
     </row>
     <row r="996" spans="1:6">
@@ -20447,16 +20447,16 @@
         <v>50</v>
       </c>
       <c r="C996" t="n">
-        <v>30043610279.125</v>
+        <v>30070223629.09224</v>
       </c>
       <c r="D996" t="n">
-        <v>103269927.14</v>
+        <v>103269744.75</v>
       </c>
       <c r="E996" t="n">
-        <v>290.923128457288</v>
+        <v>291.1813494057488</v>
       </c>
       <c r="F996" t="n">
-        <v>641.3691289969372</v>
+        <v>641.9384028999139</v>
       </c>
     </row>
     <row r="997" spans="1:6">
@@ -20467,16 +20467,16 @@
         <v>51</v>
       </c>
       <c r="C997" t="n">
-        <v>3412102.735</v>
+        <v>3437106.396740025</v>
       </c>
       <c r="D997" t="n">
         <v>2330291</v>
       </c>
       <c r="E997" t="n">
-        <v>1.46423890192255</v>
+        <v>1.474968747139317</v>
       </c>
       <c r="F997" t="n">
-        <v>3.228061083178453</v>
+        <v>3.251716099943338</v>
       </c>
     </row>
     <row r="998" spans="1:6">
@@ -20487,16 +20487,16 @@
         <v>52</v>
       </c>
       <c r="C998" t="n">
-        <v>11174172620.94</v>
+        <v>11486621093.24664</v>
       </c>
       <c r="D998" t="n">
         <v>116364402.01</v>
       </c>
       <c r="E998" t="n">
-        <v>96.0274141225744</v>
+        <v>98.71250051419949</v>
       </c>
       <c r="F998" t="n">
-        <v>211.7020371746275</v>
+        <v>217.6215786336042</v>
       </c>
     </row>
     <row r="999" spans="1:6">
@@ -20507,16 +20507,16 @@
         <v>53</v>
       </c>
       <c r="C999" t="n">
-        <v>31329690492.265</v>
+        <v>32908143414.85419</v>
       </c>
       <c r="D999" t="n">
         <v>61578043.54000001</v>
       </c>
       <c r="E999" t="n">
-        <v>508.780219233724</v>
+        <v>534.4135916477703</v>
       </c>
       <c r="F999" t="n">
-        <v>1121.656871322668</v>
+        <v>1178.168204146674</v>
       </c>
     </row>
     <row r="1000" spans="1:6">
@@ -20527,16 +20527,16 @@
         <v>54</v>
       </c>
       <c r="C1000" t="n">
-        <v>49285391158.88</v>
+        <v>48957128896.12247</v>
       </c>
       <c r="D1000" t="n">
         <v>56676905.86</v>
       </c>
       <c r="E1000" t="n">
-        <v>869.5850701628262</v>
+        <v>863.7932532353393</v>
       </c>
       <c r="F1000" t="n">
-        <v>1917.087245680967</v>
+        <v>1904.318606082629</v>
       </c>
     </row>
     <row r="1001" spans="1:6">
@@ -20547,16 +20547,16 @@
         <v>55</v>
       </c>
       <c r="C1001" t="n">
-        <v>35642422641.785</v>
+        <v>37501350962.92379</v>
       </c>
       <c r="D1001" t="n">
         <v>42023950.27999999</v>
       </c>
       <c r="E1001" t="n">
-        <v>848.1454600127851</v>
+        <v>892.3804333732853</v>
       </c>
       <c r="F1001" t="n">
-        <v>1869.821481144186</v>
+        <v>1967.341903414745</v>
       </c>
     </row>
     <row r="1002" spans="1:6">
@@ -20587,16 +20587,16 @@
         <v>7</v>
       </c>
       <c r="C1003" t="n">
-        <v>46670123469.68501</v>
+        <v>48530158071.41943</v>
       </c>
       <c r="D1003" t="n">
         <v>142931075.94</v>
       </c>
       <c r="E1003" t="n">
-        <v>326.5218789039013</v>
+        <v>339.5353862150422</v>
       </c>
       <c r="F1003" t="n">
-        <v>719.8501342315409</v>
+        <v>748.539712449682</v>
       </c>
     </row>
     <row r="1004" spans="1:6">
@@ -20607,16 +20607,16 @@
         <v>8</v>
       </c>
       <c r="C1004" t="n">
-        <v>28643416481.48</v>
+        <v>29929586068.11368</v>
       </c>
       <c r="D1004" t="n">
         <v>60361016.62</v>
       </c>
       <c r="E1004" t="n">
-        <v>474.5350241829641</v>
+        <v>495.8429752191553</v>
       </c>
       <c r="F1004" t="n">
-        <v>1046.159914313763</v>
+        <v>1093.13542316815</v>
       </c>
     </row>
     <row r="1005" spans="1:6">
@@ -20627,16 +20627,16 @@
         <v>9</v>
       </c>
       <c r="C1005" t="n">
-        <v>34336713489.255</v>
+        <v>38643118595.93936</v>
       </c>
       <c r="D1005" t="n">
         <v>112601174.13</v>
       </c>
       <c r="E1005" t="n">
-        <v>304.9409897770042</v>
+        <v>343.1857517873234</v>
       </c>
       <c r="F1005" t="n">
-        <v>672.2729060623835</v>
+        <v>756.5873083903332</v>
       </c>
     </row>
     <row r="1006" spans="1:6">
@@ -20647,16 +20647,16 @@
         <v>10</v>
       </c>
       <c r="C1006" t="n">
-        <v>38811709877.74</v>
+        <v>41096965319.5264</v>
       </c>
       <c r="D1006" t="n">
         <v>218585139.52</v>
       </c>
       <c r="E1006" t="n">
-        <v>177.55877624146</v>
+        <v>188.0135374699895</v>
       </c>
       <c r="F1006" t="n">
-        <v>391.4460781019228</v>
+        <v>414.4946447063388</v>
       </c>
     </row>
     <row r="1007" spans="1:6">
@@ -20667,16 +20667,16 @@
         <v>11</v>
       </c>
       <c r="C1007" t="n">
-        <v>30787960601.705</v>
+        <v>31278575925.37116</v>
       </c>
       <c r="D1007" t="n">
         <v>57739940.26000001</v>
       </c>
       <c r="E1007" t="n">
-        <v>533.2177425724444</v>
+        <v>541.7147261414773</v>
       </c>
       <c r="F1007" t="n">
-        <v>1175.531835275211</v>
+        <v>1194.264285251501</v>
       </c>
     </row>
     <row r="1008" spans="1:6">
@@ -20687,16 +20687,16 @@
         <v>12</v>
       </c>
       <c r="C1008" t="n">
-        <v>10568723742.43</v>
+        <v>10445122847.93863</v>
       </c>
       <c r="D1008" t="n">
         <v>44861798.23</v>
       </c>
       <c r="E1008" t="n">
-        <v>235.5840416437538</v>
+        <v>232.8288936254403</v>
       </c>
       <c r="F1008" t="n">
-        <v>519.3685782078197</v>
+        <v>513.2945788866457</v>
       </c>
     </row>
     <row r="1009" spans="1:6">
@@ -20707,16 +20707,16 @@
         <v>13</v>
       </c>
       <c r="C1009" t="n">
-        <v>1833759871.155</v>
+        <v>1547147099.831203</v>
       </c>
       <c r="D1009" t="n">
         <v>4166311.509999999</v>
       </c>
       <c r="E1009" t="n">
-        <v>440.1398855447083</v>
+        <v>371.3469566828438</v>
       </c>
       <c r="F1009" t="n">
-        <v>970.332391671864</v>
+        <v>818.6715007029974</v>
       </c>
     </row>
     <row r="1010" spans="1:6">
@@ -20727,16 +20727,16 @@
         <v>14</v>
       </c>
       <c r="C1010" t="n">
-        <v>93697634140.06003</v>
+        <v>92477079132.44818</v>
       </c>
       <c r="D1010" t="n">
         <v>246016087.5200001</v>
       </c>
       <c r="E1010" t="n">
-        <v>380.8597847587622</v>
+        <v>375.8985034868103</v>
       </c>
       <c r="F1010" t="n">
-        <v>839.6434814791672</v>
+        <v>828.7058407870221</v>
       </c>
     </row>
     <row r="1011" spans="1:6">
@@ -20747,16 +20747,16 @@
         <v>15</v>
       </c>
       <c r="C1011" t="n">
-        <v>42039229710.535</v>
+        <v>43284387325.99299</v>
       </c>
       <c r="D1011" t="n">
         <v>126348406.18</v>
       </c>
       <c r="E1011" t="n">
-        <v>332.7246538483799</v>
+        <v>342.5796069348802</v>
       </c>
       <c r="F1011" t="n">
-        <v>733.5247718741384</v>
+        <v>755.251001448637</v>
       </c>
     </row>
     <row r="1012" spans="1:6">
@@ -20787,16 +20787,16 @@
         <v>17</v>
       </c>
       <c r="C1013" t="n">
-        <v>23247019431.655</v>
+        <v>23492341602.68859</v>
       </c>
       <c r="D1013" t="n">
         <v>66312292.44000001</v>
       </c>
       <c r="E1013" t="n">
-        <v>350.568779577167</v>
+        <v>354.2682772420314</v>
       </c>
       <c r="F1013" t="n">
-        <v>772.8639314558224</v>
+        <v>781.0198440077825</v>
       </c>
     </row>
     <row r="1014" spans="1:6">
@@ -20807,16 +20807,16 @@
         <v>18</v>
       </c>
       <c r="C1014" t="n">
-        <v>1842034858.765</v>
+        <v>1840349950.314257</v>
       </c>
       <c r="D1014" t="n">
         <v>17033247.75</v>
       </c>
       <c r="E1014" t="n">
-        <v>108.1434900613713</v>
+        <v>108.0445712600087</v>
       </c>
       <c r="F1014" t="n">
-        <v>238.4131381892992</v>
+        <v>238.1950617998151</v>
       </c>
     </row>
     <row r="1015" spans="1:6">
@@ -20827,16 +20827,16 @@
         <v>19</v>
       </c>
       <c r="C1015" t="n">
-        <v>55517671603.96001</v>
+        <v>56169453953.0377</v>
       </c>
       <c r="D1015" t="n">
         <v>182745127.28</v>
       </c>
       <c r="E1015" t="n">
-        <v>303.7983689649709</v>
+        <v>307.3649885448136</v>
       </c>
       <c r="F1015" t="n">
-        <v>669.7538842201749</v>
+        <v>677.616853745896</v>
       </c>
     </row>
     <row r="1016" spans="1:6">
@@ -20847,16 +20847,16 @@
         <v>20</v>
       </c>
       <c r="C1016" t="n">
-        <v>68756969735.06999</v>
+        <v>69078098927.78487</v>
       </c>
       <c r="D1016" t="n">
         <v>94736682.47</v>
       </c>
       <c r="E1016" t="n">
-        <v>725.7692368195717</v>
+        <v>729.1589395655652</v>
       </c>
       <c r="F1016" t="n">
-        <v>1600.030859492428</v>
+        <v>1607.503798166245</v>
       </c>
     </row>
     <row r="1017" spans="1:6">
@@ -20867,16 +20867,16 @@
         <v>21</v>
       </c>
       <c r="C1017" t="n">
-        <v>22534380953.235</v>
+        <v>21424370943.94297</v>
       </c>
       <c r="D1017" t="n">
         <v>56765338.12</v>
       </c>
       <c r="E1017" t="n">
-        <v>396.9743103722572</v>
+        <v>377.4199476915398</v>
       </c>
       <c r="F1017" t="n">
-        <v>875.1695646466782</v>
+        <v>832.0600166807687</v>
       </c>
     </row>
     <row r="1018" spans="1:6">
@@ -20887,16 +20887,16 @@
         <v>22</v>
       </c>
       <c r="C1018" t="n">
-        <v>55665569272.60501</v>
+        <v>55182279362.03317</v>
       </c>
       <c r="D1018" t="n">
         <v>70598793.46000001</v>
       </c>
       <c r="E1018" t="n">
-        <v>788.4776289292269</v>
+        <v>781.6320457841599</v>
       </c>
       <c r="F1018" t="n">
-        <v>1738.277780737374</v>
+        <v>1723.186008135759</v>
       </c>
     </row>
     <row r="1019" spans="1:6">
@@ -20907,16 +20907,16 @@
         <v>23</v>
       </c>
       <c r="C1019" t="n">
-        <v>37749002673.795</v>
+        <v>36039978056.97714</v>
       </c>
       <c r="D1019" t="n">
         <v>98324076.81000002</v>
       </c>
       <c r="E1019" t="n">
-        <v>383.9243031667677</v>
+        <v>366.5427556123436</v>
       </c>
       <c r="F1019" t="n">
-        <v>846.3995187614561</v>
+        <v>808.0801590229728</v>
       </c>
     </row>
     <row r="1020" spans="1:6">
@@ -20927,16 +20927,16 @@
         <v>24</v>
       </c>
       <c r="C1020" t="n">
-        <v>7485320801.755001</v>
+        <v>7417671512.878674</v>
       </c>
       <c r="D1020" t="n">
         <v>21786765.92</v>
       </c>
       <c r="E1020" t="n">
-        <v>343.5719110050915</v>
+        <v>340.4668476319992</v>
       </c>
       <c r="F1020" t="n">
-        <v>757.4386350018248</v>
+        <v>750.5932122895055</v>
       </c>
     </row>
     <row r="1021" spans="1:6">
@@ -20947,16 +20947,16 @@
         <v>25</v>
       </c>
       <c r="C1021" t="n">
-        <v>12463209770.485</v>
+        <v>12643330920.16602</v>
       </c>
       <c r="D1021" t="n">
         <v>40742545.86000001</v>
       </c>
       <c r="E1021" t="n">
-        <v>305.9015951853186</v>
+        <v>310.3225547959418</v>
       </c>
       <c r="F1021" t="n">
-        <v>674.3906567455534</v>
+        <v>684.1371043031334</v>
       </c>
     </row>
     <row r="1022" spans="1:6">
@@ -20967,16 +20967,16 @@
         <v>26</v>
       </c>
       <c r="C1022" t="n">
-        <v>1312255410.4</v>
+        <v>1287911685.414643</v>
       </c>
       <c r="D1022" t="n">
         <v>11072409.92</v>
       </c>
       <c r="E1022" t="n">
-        <v>118.5157901379432</v>
+        <v>116.3171969535105</v>
       </c>
       <c r="F1022" t="n">
-        <v>261.2799109381095</v>
+        <v>256.4328924037092</v>
       </c>
     </row>
     <row r="1023" spans="1:6">
@@ -20987,16 +20987,16 @@
         <v>27</v>
       </c>
       <c r="C1023" t="n">
-        <v>52853515864.855</v>
+        <v>52232948303.11605</v>
       </c>
       <c r="D1023" t="n">
         <v>116233454.98</v>
       </c>
       <c r="E1023" t="n">
-        <v>454.7186167179611</v>
+        <v>449.3796412754284</v>
       </c>
       <c r="F1023" t="n">
-        <v>1002.472662416417</v>
+        <v>990.7023571558095</v>
       </c>
     </row>
     <row r="1024" spans="1:6">
@@ -21007,16 +21007,16 @@
         <v>28</v>
       </c>
       <c r="C1024" t="n">
-        <v>20788697467.79</v>
+        <v>21717990904.23017</v>
       </c>
       <c r="D1024" t="n">
         <v>59791646.17</v>
       </c>
       <c r="E1024" t="n">
-        <v>347.6856517494675</v>
+        <v>363.2278469550986</v>
       </c>
       <c r="F1024" t="n">
-        <v>766.507787846876</v>
+        <v>800.7721113972106</v>
       </c>
     </row>
     <row r="1025" spans="1:6">
@@ -21027,16 +21027,16 @@
         <v>29</v>
       </c>
       <c r="C1025" t="n">
-        <v>59359559836.175</v>
+        <v>57381702052.25567</v>
       </c>
       <c r="D1025" t="n">
         <v>78237002.67</v>
       </c>
       <c r="E1025" t="n">
-        <v>758.7146466557625</v>
+        <v>733.434309776526</v>
       </c>
       <c r="F1025" t="n">
-        <v>1672.662310017294</v>
+        <v>1616.929279333329</v>
       </c>
     </row>
     <row r="1026" spans="1:6">
@@ -21047,16 +21047,16 @@
         <v>30</v>
       </c>
       <c r="C1026" t="n">
-        <v>25622631586.04</v>
+        <v>26003987898.54591</v>
       </c>
       <c r="D1026" t="n">
         <v>68717185.59999999</v>
       </c>
       <c r="E1026" t="n">
-        <v>372.8707944354462</v>
+        <v>378.4204441944711</v>
       </c>
       <c r="F1026" t="n">
-        <v>822.0309534123847</v>
+        <v>834.265711271131</v>
       </c>
     </row>
     <row r="1027" spans="1:6">
@@ -21067,16 +21067,16 @@
         <v>31</v>
       </c>
       <c r="C1027" t="n">
-        <v>11813857238.25</v>
+        <v>11366354677.32653</v>
       </c>
       <c r="D1027" t="n">
         <v>24493939.66</v>
       </c>
       <c r="E1027" t="n">
-        <v>482.3175610880884</v>
+        <v>464.0476311733728</v>
       </c>
       <c r="F1027" t="n">
-        <v>1063.3172951748</v>
+        <v>1023.039407684818</v>
       </c>
     </row>
     <row r="1028" spans="1:6">
@@ -21087,16 +21087,16 @@
         <v>32</v>
       </c>
       <c r="C1028" t="n">
-        <v>39613667027.21999</v>
+        <v>39129905457.10504</v>
       </c>
       <c r="D1028" t="n">
         <v>131705786.52</v>
       </c>
       <c r="E1028" t="n">
-        <v>300.7739300900383</v>
+        <v>297.1008828922108</v>
       </c>
       <c r="F1028" t="n">
-        <v>663.0862062764985</v>
+        <v>654.988606424168</v>
       </c>
     </row>
     <row r="1029" spans="1:6">
@@ -21107,16 +21107,16 @@
         <v>33</v>
       </c>
       <c r="C1029" t="n">
-        <v>26140850667.105</v>
+        <v>26670022529.78182</v>
       </c>
       <c r="D1029" t="n">
         <v>42703525.56999999</v>
       </c>
       <c r="E1029" t="n">
-        <v>612.1473653095619</v>
+        <v>624.5391258401859</v>
       </c>
       <c r="F1029" t="n">
-        <v>1349.54008156146</v>
+        <v>1376.858956827274</v>
       </c>
     </row>
     <row r="1030" spans="1:6">
@@ -21127,16 +21127,16 @@
         <v>34</v>
       </c>
       <c r="C1030" t="n">
-        <v>20612310764.615</v>
+        <v>19720934884.99102</v>
       </c>
       <c r="D1030" t="n">
         <v>38599660.71</v>
       </c>
       <c r="E1030" t="n">
-        <v>534.002382028062</v>
+        <v>510.9095396758741</v>
       </c>
       <c r="F1030" t="n">
-        <v>1177.261651419066</v>
+        <v>1126.351171169432</v>
       </c>
     </row>
     <row r="1031" spans="1:6">
@@ -21147,16 +21147,16 @@
         <v>35</v>
       </c>
       <c r="C1031" t="n">
-        <v>2218544448.24</v>
+        <v>2195952032.451259</v>
       </c>
       <c r="D1031" t="n">
         <v>17621002.87</v>
       </c>
       <c r="E1031" t="n">
-        <v>125.9034156345949</v>
+        <v>124.6212856698354</v>
       </c>
       <c r="F1031" t="n">
-        <v>277.566670108028</v>
+        <v>274.7400863877191</v>
       </c>
     </row>
     <row r="1032" spans="1:6">
@@ -21167,16 +21167,16 @@
         <v>36</v>
       </c>
       <c r="C1032" t="n">
-        <v>13462032651.895</v>
+        <v>13606267655.00595</v>
       </c>
       <c r="D1032" t="n">
         <v>64052323.05999999</v>
       </c>
       <c r="E1032" t="n">
-        <v>210.1724341720542</v>
+        <v>212.4242651162003</v>
       </c>
       <c r="F1032" t="n">
-        <v>463.3461483757108</v>
+        <v>468.3105348751752</v>
       </c>
     </row>
     <row r="1033" spans="1:6">
@@ -21187,16 +21187,16 @@
         <v>37</v>
       </c>
       <c r="C1033" t="n">
-        <v>17145836760.14</v>
+        <v>17954856943.07486</v>
       </c>
       <c r="D1033" t="n">
         <v>35551998.8</v>
       </c>
       <c r="E1033" t="n">
-        <v>482.27490264598</v>
+        <v>505.0308716559379</v>
       </c>
       <c r="F1033" t="n">
-        <v>1063.223250373328</v>
+        <v>1113.391059652681</v>
       </c>
     </row>
     <row r="1034" spans="1:6">
@@ -21207,16 +21207,16 @@
         <v>38</v>
       </c>
       <c r="C1034" t="n">
-        <v>13762614837.76</v>
+        <v>13622148093.59575</v>
       </c>
       <c r="D1034" t="n">
         <v>43119865.39</v>
       </c>
       <c r="E1034" t="n">
-        <v>319.1710992899275</v>
+        <v>315.9135115657131</v>
       </c>
       <c r="F1034" t="n">
-        <v>703.6446054945742</v>
+        <v>696.4629275977711</v>
       </c>
     </row>
     <row r="1035" spans="1:6">
@@ -21227,16 +21227,16 @@
         <v>39</v>
       </c>
       <c r="C1035" t="n">
-        <v>26247480069.54</v>
+        <v>27371116839.49265</v>
       </c>
       <c r="D1035" t="n">
         <v>127908265.29</v>
       </c>
       <c r="E1035" t="n">
-        <v>205.2055041949823</v>
+        <v>213.9902122621668</v>
       </c>
       <c r="F1035" t="n">
-        <v>452.396054548258</v>
+        <v>471.762821953173</v>
       </c>
     </row>
     <row r="1036" spans="1:6">
@@ -21247,16 +21247,16 @@
         <v>40</v>
       </c>
       <c r="C1036" t="n">
-        <v>66925324233.01501</v>
+        <v>68285479178.258</v>
       </c>
       <c r="D1036" t="n">
         <v>123493023.42</v>
       </c>
       <c r="E1036" t="n">
-        <v>541.9360736306686</v>
+        <v>552.9500961849396</v>
       </c>
       <c r="F1036" t="n">
-        <v>1194.752267926172</v>
+        <v>1219.033782049318</v>
       </c>
     </row>
     <row r="1037" spans="1:6">
@@ -21267,16 +21267,16 @@
         <v>41</v>
       </c>
       <c r="C1037" t="n">
-        <v>26408867724.945</v>
+        <v>27469083037.69395</v>
       </c>
       <c r="D1037" t="n">
         <v>80611445.53</v>
       </c>
       <c r="E1037" t="n">
-        <v>327.6069241943663</v>
+        <v>340.7590926709182</v>
       </c>
       <c r="F1037" t="n">
-        <v>722.2422250789001</v>
+        <v>751.2374957023063</v>
       </c>
     </row>
     <row r="1038" spans="1:6">
@@ -21287,16 +21287,16 @@
         <v>42</v>
       </c>
       <c r="C1038" t="n">
-        <v>7865481925.445001</v>
+        <v>8494601431.178171</v>
       </c>
       <c r="D1038" t="n">
         <v>61385612.4</v>
       </c>
       <c r="E1038" t="n">
-        <v>128.1323361929187</v>
+        <v>138.3809837364785</v>
       </c>
       <c r="F1038" t="n">
-        <v>282.4805483709087</v>
+        <v>305.0747167454405</v>
       </c>
     </row>
     <row r="1039" spans="1:6">
@@ -21307,16 +21307,16 @@
         <v>43</v>
       </c>
       <c r="C1039" t="n">
-        <v>78555762958.50499</v>
+        <v>79253817679.92491</v>
       </c>
       <c r="D1039" t="n">
         <v>242280186.46</v>
       </c>
       <c r="E1039" t="n">
-        <v>324.2351927588367</v>
+        <v>327.1163805753863</v>
       </c>
       <c r="F1039" t="n">
-        <v>714.8089059561313</v>
+        <v>721.1607726164967</v>
       </c>
     </row>
     <row r="1040" spans="1:6">
@@ -21327,16 +21327,16 @@
         <v>44</v>
       </c>
       <c r="C1040" t="n">
-        <v>3162047553.255</v>
+        <v>3193580771.70115</v>
       </c>
       <c r="D1040" t="n">
         <v>8406030.800000001</v>
       </c>
       <c r="E1040" t="n">
-        <v>376.1641645727731</v>
+        <v>379.915425922678</v>
       </c>
       <c r="F1040" t="n">
-        <v>829.2915172171357</v>
+        <v>837.561547989136</v>
       </c>
     </row>
     <row r="1041" spans="1:6">
@@ -21347,16 +21347,16 @@
         <v>45</v>
       </c>
       <c r="C1041" t="n">
-        <v>24126688192.45</v>
+        <v>25170131440.98152</v>
       </c>
       <c r="D1041" t="n">
         <v>100287569.93</v>
       </c>
       <c r="E1041" t="n">
-        <v>240.5750603917341</v>
+        <v>250.9795726284932</v>
       </c>
       <c r="F1041" t="n">
-        <v>530.3717781396169</v>
+        <v>553.3095658167761</v>
       </c>
     </row>
     <row r="1042" spans="1:6">
@@ -21367,16 +21367,16 @@
         <v>46</v>
       </c>
       <c r="C1042" t="n">
-        <v>2297033611.135</v>
+        <v>2413110543.999428</v>
       </c>
       <c r="D1042" t="n">
         <v>17766241.46</v>
       </c>
       <c r="E1042" t="n">
-        <v>129.2920405425471</v>
+        <v>135.8256077647291</v>
       </c>
       <c r="F1042" t="n">
-        <v>285.0372325800993</v>
+        <v>299.4411348781219</v>
       </c>
     </row>
     <row r="1043" spans="1:6">
@@ -21387,16 +21387,16 @@
         <v>47</v>
       </c>
       <c r="C1043" t="n">
-        <v>24309127592.29</v>
+        <v>24786446201.82143</v>
       </c>
       <c r="D1043" t="n">
         <v>81520552.23999999</v>
       </c>
       <c r="E1043" t="n">
-        <v>298.1963066285774</v>
+        <v>304.0515001523673</v>
       </c>
       <c r="F1043" t="n">
-        <v>657.4035775933618</v>
+        <v>670.3119372359091</v>
       </c>
     </row>
     <row r="1044" spans="1:6">
@@ -21407,16 +21407,16 @@
         <v>48</v>
       </c>
       <c r="C1044" t="n">
-        <v>186716651073.555</v>
+        <v>187552845865.9333</v>
       </c>
       <c r="D1044" t="n">
         <v>485776771.1</v>
       </c>
       <c r="E1044" t="n">
-        <v>384.367187115084</v>
+        <v>386.0885431825731</v>
       </c>
       <c r="F1044" t="n">
-        <v>847.3759007139142</v>
+        <v>851.1708023003006</v>
       </c>
     </row>
     <row r="1045" spans="1:6">
@@ -21427,16 +21427,16 @@
         <v>49</v>
       </c>
       <c r="C1045" t="n">
-        <v>29418461566.57</v>
+        <v>29562969722.14373</v>
       </c>
       <c r="D1045" t="n">
         <v>43310687.55999999</v>
       </c>
       <c r="E1045" t="n">
-        <v>679.2425432132761</v>
+        <v>682.5790904655806</v>
       </c>
       <c r="F1045" t="n">
-        <v>1497.458110767989</v>
+        <v>1504.813862840419</v>
       </c>
     </row>
     <row r="1046" spans="1:6">
@@ -21447,16 +21447,16 @@
         <v>50</v>
       </c>
       <c r="C1046" t="n">
-        <v>25757214216.315</v>
+        <v>25978341270.06553</v>
       </c>
       <c r="D1046" t="n">
         <v>94604496.53</v>
       </c>
       <c r="E1046" t="n">
-        <v>272.2620505479583</v>
+        <v>274.5994347301192</v>
       </c>
       <c r="F1046" t="n">
-        <v>600.2289166380289</v>
+        <v>605.3819138060209</v>
       </c>
     </row>
     <row r="1047" spans="1:6">
@@ -21467,16 +21467,16 @@
         <v>51</v>
       </c>
       <c r="C1047" t="n">
-        <v>666761.1900000003</v>
+        <v>944527.4533046795</v>
       </c>
       <c r="D1047" t="n">
         <v>2330902.49</v>
       </c>
       <c r="E1047" t="n">
-        <v>0.2860528026635727</v>
+        <v>0.4052196337499642</v>
       </c>
       <c r="F1047" t="n">
-        <v>0.6306320087521126</v>
+        <v>0.893347204565171</v>
       </c>
     </row>
     <row r="1048" spans="1:6">
@@ -21487,16 +21487,16 @@
         <v>52</v>
       </c>
       <c r="C1048" t="n">
-        <v>9854382555.039999</v>
+        <v>9780201502.579603</v>
       </c>
       <c r="D1048" t="n">
         <v>109423739.94</v>
       </c>
       <c r="E1048" t="n">
-        <v>90.05708048768416</v>
+        <v>89.3791558206871</v>
       </c>
       <c r="F1048" t="n">
-        <v>198.5398396431485</v>
+        <v>197.0452869222868</v>
       </c>
     </row>
     <row r="1049" spans="1:6">
@@ -21507,16 +21507,16 @@
         <v>53</v>
       </c>
       <c r="C1049" t="n">
-        <v>34906548902.68999</v>
+        <v>36907207628.77538</v>
       </c>
       <c r="D1049" t="n">
         <v>65643767.64000001</v>
       </c>
       <c r="E1049" t="n">
-        <v>531.7572430352047</v>
+        <v>562.2347551892494</v>
       </c>
       <c r="F1049" t="n">
-        <v>1172.312017995412</v>
+        <v>1239.502741290219</v>
       </c>
     </row>
     <row r="1050" spans="1:6">
@@ -21527,16 +21527,16 @@
         <v>54</v>
       </c>
       <c r="C1050" t="n">
-        <v>57537593503.22499</v>
+        <v>57879053852.35606</v>
       </c>
       <c r="D1050" t="n">
         <v>65646255.15</v>
       </c>
       <c r="E1050" t="n">
-        <v>876.4794483973698</v>
+        <v>881.6809690073549</v>
       </c>
       <c r="F1050" t="n">
-        <v>1932.286591936841</v>
+        <v>1943.753864273615</v>
       </c>
     </row>
     <row r="1051" spans="1:6">
@@ -21547,16 +21547,16 @@
         <v>55</v>
       </c>
       <c r="C1051" t="n">
-        <v>34325800769.71</v>
+        <v>35825589136.60789</v>
       </c>
       <c r="D1051" t="n">
         <v>43668476.54000001</v>
       </c>
       <c r="E1051" t="n">
-        <v>786.0544605504572</v>
+        <v>820.399335520485</v>
       </c>
       <c r="F1051" t="n">
-        <v>1732.935663729538</v>
+        <v>1808.652375088461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>